<commit_message>
Add Burdekin dataset and clean up soil water at Narrabri
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/Narrabri0203Observed.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/Narrabri0203Observed.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED61F11-9C06-46BF-AAB2-9DED770AE8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43ED442-5FD9-4869-A25A-0A55976329FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$FJ$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$EV$44</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="166">
   <si>
     <t>SimulationName</t>
   </si>
@@ -305,12 +305,6 @@
     <t>Depth(3)</t>
   </si>
   <si>
-    <t>TotalWaterMM</t>
-  </si>
-  <si>
-    <t>SW2400mm</t>
-  </si>
-  <si>
     <t>Cotton.Phenology.CutoutDAS</t>
   </si>
   <si>
@@ -500,69 +494,6 @@
     <t>Cotton.SeedCotton.Wt</t>
   </si>
   <si>
-    <t>Soil.Water.Volumetric(1)</t>
-  </si>
-  <si>
-    <t>Soil.Water.Volumetric(2)</t>
-  </si>
-  <si>
-    <t>Soil.Water.Volumetric(3)</t>
-  </si>
-  <si>
-    <t>Soil.Water.Volumetric(4)</t>
-  </si>
-  <si>
-    <t>Soil.Water.Volumetric(5)</t>
-  </si>
-  <si>
-    <t>Soil.Water.Volumetric(6)</t>
-  </si>
-  <si>
-    <t>Soil.Water.Volumetric(7)</t>
-  </si>
-  <si>
-    <t>Soil.Water.Volumetric(8)</t>
-  </si>
-  <si>
-    <t>Soil.Water.Volumetric(9)</t>
-  </si>
-  <si>
-    <t>Soil.Water.Volumetric(10)</t>
-  </si>
-  <si>
-    <t>Soil.Water.Volumetric(11)</t>
-  </si>
-  <si>
-    <t>Soil.Water.Volumetric(12)</t>
-  </si>
-  <si>
-    <t>Soil.Water.MM(1)</t>
-  </si>
-  <si>
-    <t>Soil.Water.MM(2)</t>
-  </si>
-  <si>
-    <t>Soil.Water.MM(3)</t>
-  </si>
-  <si>
-    <t>Soil.Water.MM(4)</t>
-  </si>
-  <si>
-    <t>Soil.Water.MM(5)</t>
-  </si>
-  <si>
-    <t>Soil.Water.MM(6)</t>
-  </si>
-  <si>
-    <t>Soil.Water.MM(7)</t>
-  </si>
-  <si>
-    <t>Soil.Water.MM(8)</t>
-  </si>
-  <si>
-    <t>Soil.Water.MM(9)</t>
-  </si>
-  <si>
     <t>Soil.Water.MM(10)</t>
   </si>
   <si>
@@ -572,10 +503,37 @@
     <t>Soil.Water.MM(12)</t>
   </si>
   <si>
-    <t>TotalSW180cm</t>
-  </si>
-  <si>
     <t>Narrabri0203RowSpacing1m</t>
+  </si>
+  <si>
+    <t>Soil.Water.PAWmm(1)</t>
+  </si>
+  <si>
+    <t>Soil.Water.PAWmm(2)</t>
+  </si>
+  <si>
+    <t>Soil.Water.PAWmm(3)</t>
+  </si>
+  <si>
+    <t>Soil.Water.PAWmm(4)</t>
+  </si>
+  <si>
+    <t>Soil.Water.PAWmm(5)</t>
+  </si>
+  <si>
+    <t>Soil.Water.PAWmm(6)</t>
+  </si>
+  <si>
+    <t>Soil.Water.PAWmm(7)</t>
+  </si>
+  <si>
+    <t>Soil.Water.PAWmm(8)</t>
+  </si>
+  <si>
+    <t>Soil.Water.PAWmm(9)</t>
+  </si>
+  <si>
+    <t>TotalPAWmm</t>
   </si>
 </sst>
 </file>
@@ -587,19 +545,13 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -647,7 +599,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -656,11 +608,11 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -977,13 +929,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:FJ44"/>
+  <dimension ref="A1:EV44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="CN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="CO2" sqref="CO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1079,72 +1031,59 @@
     <col min="91" max="91" width="12" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="11.73046875" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="94" max="95" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="22" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="12" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="22" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="12" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="12" bestFit="1" customWidth="1"/>
     <col min="100" max="100" width="11.1328125" bestFit="1" customWidth="1"/>
     <col min="101" max="101" width="12" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="22" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="12" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="22" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="12" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="12" bestFit="1" customWidth="1"/>
     <col min="106" max="106" width="11.1328125" bestFit="1" customWidth="1"/>
     <col min="107" max="107" width="12" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="22" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="12" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="22" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="12" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="22" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="12" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="22" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="12" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="22" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="12" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="23" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="13" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="23" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="13" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="23" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="13" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="7.1328125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="12" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="12" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="13" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="13" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="13" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="7.1328125" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="18.265625" bestFit="1" customWidth="1"/>
     <col min="133" max="133" width="18.1328125" bestFit="1" customWidth="1"/>
     <col min="134" max="134" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="145" max="145" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="7" bestFit="1" customWidth="1"/>
-    <col min="150" max="157" width="18" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="5.86328125" bestFit="1" customWidth="1"/>
-    <col min="159" max="166" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="7" bestFit="1" customWidth="1"/>
+    <col min="136" max="143" width="18" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="5.86328125" bestFit="1" customWidth="1"/>
+    <col min="145" max="152" width="23.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:166" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:152" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1165,13 +1104,13 @@
         <v>3</v>
       </c>
       <c r="I1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1" t="s">
         <v>92</v>
-      </c>
-      <c r="J1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K1" t="s">
-        <v>94</v>
       </c>
       <c r="L1" t="s">
         <v>51</v>
@@ -1183,10 +1122,10 @@
         <v>63</v>
       </c>
       <c r="O1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="Q1" t="s">
         <v>52</v>
@@ -1198,7 +1137,7 @@
         <v>53</v>
       </c>
       <c r="T1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="U1" t="s">
         <v>68</v>
@@ -1207,7 +1146,7 @@
         <v>54</v>
       </c>
       <c r="W1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="X1" t="s">
         <v>15</v>
@@ -1234,16 +1173,16 @@
         <v>77</v>
       </c>
       <c r="AF1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG1" t="s">
         <v>139</v>
       </c>
-      <c r="AG1" t="s">
-        <v>141</v>
-      </c>
       <c r="AH1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AI1" t="s">
         <v>140</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>142</v>
       </c>
       <c r="AJ1" t="s">
         <v>57</v>
@@ -1252,22 +1191,22 @@
         <v>59</v>
       </c>
       <c r="AL1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AM1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AN1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AO1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AP1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AQ1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AR1" t="s">
         <v>58</v>
@@ -1276,52 +1215,52 @@
         <v>78</v>
       </c>
       <c r="AT1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AU1" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="AV1" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="AW1" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AY1" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="AV1" s="11" t="s">
+      <c r="AZ1" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="BA1" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="BB1" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="AW1" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="AX1" t="s">
+      <c r="BC1" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="BD1" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="BE1" t="s">
         <v>101</v>
       </c>
-      <c r="AY1" s="11" t="s">
+      <c r="BF1" t="s">
         <v>102</v>
       </c>
-      <c r="AZ1" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="BA1" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="BB1" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="BC1" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="BD1" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="BE1" t="s">
+      <c r="BG1" t="s">
         <v>103</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>104</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>105</v>
       </c>
       <c r="BH1" t="s">
         <v>74</v>
       </c>
       <c r="BI1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="BJ1" t="s">
         <v>76</v>
@@ -1330,49 +1269,49 @@
         <v>60</v>
       </c>
       <c r="BL1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="BM1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="BN1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="BO1" t="s">
         <v>9</v>
       </c>
       <c r="BP1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>128</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>150</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>149</v>
+      </c>
+      <c r="BT1" t="s">
         <v>107</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BU1" t="s">
+        <v>129</v>
+      </c>
+      <c r="BV1" t="s">
         <v>130</v>
       </c>
-      <c r="BR1" t="s">
-        <v>152</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>151</v>
-      </c>
-      <c r="BT1" t="s">
+      <c r="BW1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BY1" t="s">
         <v>109</v>
       </c>
-      <c r="BU1" t="s">
-        <v>131</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>132</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>114</v>
-      </c>
-      <c r="BX1" t="s">
+      <c r="BZ1" t="s">
         <v>110</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>112</v>
       </c>
       <c r="CA1" t="s">
         <v>75</v>
@@ -1390,13 +1329,13 @@
         <v>7</v>
       </c>
       <c r="CF1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="CG1" t="s">
         <v>8</v>
       </c>
       <c r="CH1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="CI1" t="s">
         <v>49</v>
@@ -1411,240 +1350,198 @@
         <v>65</v>
       </c>
       <c r="CM1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="CN1" t="s">
         <v>66</v>
       </c>
       <c r="CO1" t="s">
-        <v>89</v>
+        <v>165</v>
       </c>
       <c r="CP1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="CQ1" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="CR1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>157</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>88</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>158</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>87</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>159</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>86</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>160</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>93</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>161</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>94</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>162</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>85</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>163</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>84</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>164</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>83</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>152</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>82</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>153</v>
+      </c>
+      <c r="DL1" t="s">
+        <v>81</v>
+      </c>
+      <c r="DM1" t="s">
         <v>154</v>
       </c>
-      <c r="CS1" t="s">
-        <v>79</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>166</v>
-      </c>
-      <c r="CU1" t="s">
+      <c r="DN1" t="s">
+        <v>44</v>
+      </c>
+      <c r="DO1" t="s">
+        <v>20</v>
+      </c>
+      <c r="DP1" t="s">
+        <v>113</v>
+      </c>
+      <c r="DQ1" t="s">
+        <v>21</v>
+      </c>
+      <c r="DR1" t="s">
+        <v>114</v>
+      </c>
+      <c r="DS1" t="s">
+        <v>22</v>
+      </c>
+      <c r="DT1" t="s">
+        <v>115</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DV1" t="s">
+        <v>116</v>
+      </c>
+      <c r="DW1" t="s">
+        <v>24</v>
+      </c>
+      <c r="DX1" t="s">
+        <v>117</v>
+      </c>
+      <c r="DY1" t="s">
+        <v>25</v>
+      </c>
+      <c r="DZ1" t="s">
+        <v>118</v>
+      </c>
+      <c r="EA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="EB1" t="s">
+        <v>119</v>
+      </c>
+      <c r="EC1" t="s">
+        <v>27</v>
+      </c>
+      <c r="ED1" t="s">
+        <v>120</v>
+      </c>
+      <c r="EE1" t="s">
+        <v>45</v>
+      </c>
+      <c r="EF1" t="s">
+        <v>28</v>
+      </c>
+      <c r="EG1" t="s">
+        <v>29</v>
+      </c>
+      <c r="EH1" t="s">
+        <v>30</v>
+      </c>
+      <c r="EI1" t="s">
+        <v>31</v>
+      </c>
+      <c r="EJ1" t="s">
+        <v>32</v>
+      </c>
+      <c r="EK1" t="s">
+        <v>33</v>
+      </c>
+      <c r="EL1" t="s">
+        <v>34</v>
+      </c>
+      <c r="EM1" t="s">
+        <v>35</v>
+      </c>
+      <c r="EN1" t="s">
+        <v>46</v>
+      </c>
+      <c r="EO1" t="s">
+        <v>36</v>
+      </c>
+      <c r="EP1" t="s">
+        <v>37</v>
+      </c>
+      <c r="EQ1" t="s">
+        <v>38</v>
+      </c>
+      <c r="ER1" t="s">
+        <v>39</v>
+      </c>
+      <c r="ES1" t="s">
+        <v>40</v>
+      </c>
+      <c r="ET1" t="s">
+        <v>41</v>
+      </c>
+      <c r="EU1" t="s">
+        <v>42</v>
+      </c>
+      <c r="EV1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:152" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>155</v>
       </c>
-      <c r="CV1" t="s">
-        <v>80</v>
-      </c>
-      <c r="CW1" t="s">
-        <v>167</v>
-      </c>
-      <c r="CX1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CY1" t="s">
-        <v>88</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>168</v>
-      </c>
-      <c r="DA1" t="s">
-        <v>157</v>
-      </c>
-      <c r="DB1" t="s">
-        <v>87</v>
-      </c>
-      <c r="DC1" t="s">
-        <v>169</v>
-      </c>
-      <c r="DD1" t="s">
-        <v>158</v>
-      </c>
-      <c r="DE1" t="s">
-        <v>86</v>
-      </c>
-      <c r="DF1" t="s">
-        <v>170</v>
-      </c>
-      <c r="DG1" t="s">
-        <v>159</v>
-      </c>
-      <c r="DH1" t="s">
-        <v>95</v>
-      </c>
-      <c r="DI1" t="s">
-        <v>171</v>
-      </c>
-      <c r="DJ1" t="s">
-        <v>160</v>
-      </c>
-      <c r="DK1" t="s">
-        <v>96</v>
-      </c>
-      <c r="DL1" t="s">
-        <v>172</v>
-      </c>
-      <c r="DM1" t="s">
-        <v>161</v>
-      </c>
-      <c r="DN1" t="s">
-        <v>85</v>
-      </c>
-      <c r="DO1" t="s">
-        <v>173</v>
-      </c>
-      <c r="DP1" t="s">
-        <v>162</v>
-      </c>
-      <c r="DQ1" t="s">
-        <v>84</v>
-      </c>
-      <c r="DR1" t="s">
-        <v>174</v>
-      </c>
-      <c r="DS1" t="s">
-        <v>163</v>
-      </c>
-      <c r="DT1" t="s">
-        <v>83</v>
-      </c>
-      <c r="DU1" t="s">
-        <v>175</v>
-      </c>
-      <c r="DV1" t="s">
-        <v>164</v>
-      </c>
-      <c r="DW1" t="s">
-        <v>82</v>
-      </c>
-      <c r="DX1" t="s">
-        <v>176</v>
-      </c>
-      <c r="DY1" t="s">
-        <v>165</v>
-      </c>
-      <c r="DZ1" t="s">
-        <v>81</v>
-      </c>
-      <c r="EA1" t="s">
-        <v>177</v>
-      </c>
-      <c r="EB1" t="s">
-        <v>44</v>
-      </c>
-      <c r="EC1" t="s">
-        <v>20</v>
-      </c>
-      <c r="ED1" t="s">
-        <v>115</v>
-      </c>
-      <c r="EE1" t="s">
-        <v>21</v>
-      </c>
-      <c r="EF1" t="s">
-        <v>116</v>
-      </c>
-      <c r="EG1" t="s">
-        <v>22</v>
-      </c>
-      <c r="EH1" t="s">
-        <v>117</v>
-      </c>
-      <c r="EI1" t="s">
-        <v>23</v>
-      </c>
-      <c r="EJ1" t="s">
-        <v>118</v>
-      </c>
-      <c r="EK1" t="s">
-        <v>24</v>
-      </c>
-      <c r="EL1" t="s">
-        <v>119</v>
-      </c>
-      <c r="EM1" t="s">
-        <v>25</v>
-      </c>
-      <c r="EN1" t="s">
-        <v>120</v>
-      </c>
-      <c r="EO1" t="s">
-        <v>26</v>
-      </c>
-      <c r="EP1" t="s">
-        <v>121</v>
-      </c>
-      <c r="EQ1" t="s">
-        <v>27</v>
-      </c>
-      <c r="ER1" t="s">
-        <v>122</v>
-      </c>
-      <c r="ES1" t="s">
-        <v>45</v>
-      </c>
-      <c r="ET1" t="s">
-        <v>28</v>
-      </c>
-      <c r="EU1" t="s">
-        <v>29</v>
-      </c>
-      <c r="EV1" t="s">
-        <v>30</v>
-      </c>
-      <c r="EW1" t="s">
-        <v>31</v>
-      </c>
-      <c r="EX1" t="s">
-        <v>32</v>
-      </c>
-      <c r="EY1" t="s">
-        <v>33</v>
-      </c>
-      <c r="EZ1" t="s">
-        <v>34</v>
-      </c>
-      <c r="FA1" t="s">
-        <v>35</v>
-      </c>
-      <c r="FB1" t="s">
-        <v>46</v>
-      </c>
-      <c r="FC1" t="s">
-        <v>36</v>
-      </c>
-      <c r="FD1" t="s">
-        <v>37</v>
-      </c>
-      <c r="FE1" t="s">
-        <v>38</v>
-      </c>
-      <c r="FF1" t="s">
-        <v>39</v>
-      </c>
-      <c r="FG1" t="s">
-        <v>40</v>
-      </c>
-      <c r="FH1" t="s">
-        <v>41</v>
-      </c>
-      <c r="FI1" t="s">
-        <v>42</v>
-      </c>
-      <c r="FJ1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:166" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>179</v>
-      </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C2" s="7">
         <v>37530</v>
@@ -1656,7 +1553,7 @@
         <v>-9</v>
       </c>
       <c r="H2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I2" s="6">
         <v>12</v>
@@ -1690,37 +1587,37 @@
       <c r="BX2" s="4"/>
       <c r="BY2" s="4"/>
       <c r="BZ2" s="4"/>
-      <c r="EB2">
+      <c r="DN2">
         <v>52.5</v>
       </c>
-      <c r="EC2">
+      <c r="DO2">
         <v>37.5</v>
       </c>
-      <c r="EE2">
+      <c r="DQ2">
         <v>11</v>
       </c>
-      <c r="EG2">
+      <c r="DS2">
         <v>2</v>
       </c>
-      <c r="EI2">
+      <c r="DU2">
         <v>0.5</v>
       </c>
-      <c r="EK2">
+      <c r="DW2">
         <v>0.5</v>
       </c>
-      <c r="EM2">
+      <c r="DY2">
         <v>0.5</v>
       </c>
-      <c r="EO2">
+      <c r="EA2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:166" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:152" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C3" s="7">
         <v>37539</v>
@@ -1738,7 +1635,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I3" s="6">
         <v>12</v>
@@ -1786,12 +1683,12 @@
       <c r="CD3" s="4"/>
       <c r="CJ3" s="4"/>
     </row>
-    <row r="4" spans="1:166" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:152" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C4" s="7">
         <v>37592</v>
@@ -1809,7 +1706,7 @@
         <v>53</v>
       </c>
       <c r="H4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I4" s="6">
         <v>12</v>
@@ -1860,12 +1757,12 @@
       <c r="CD4" s="4"/>
       <c r="CJ4" s="4"/>
     </row>
-    <row r="5" spans="1:166" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:152" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C5" s="7">
         <v>37594</v>
@@ -1874,7 +1771,7 @@
         <v>55</v>
       </c>
       <c r="H5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I5" s="6">
         <v>12</v>
@@ -1970,12 +1867,12 @@
       </c>
       <c r="CJ5" s="4"/>
     </row>
-    <row r="6" spans="1:166" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:152" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C6" s="7">
         <v>37595</v>
@@ -1984,7 +1881,7 @@
         <v>56</v>
       </c>
       <c r="H6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I6" s="6">
         <v>12</v>
@@ -2019,12 +1916,12 @@
       <c r="BM6" s="6"/>
       <c r="BN6" s="6"/>
     </row>
-    <row r="7" spans="1:166" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:152" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C7" s="7">
         <v>37599</v>
@@ -2033,7 +1930,7 @@
         <v>60</v>
       </c>
       <c r="H7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I7" s="6">
         <v>12</v>
@@ -2066,70 +1963,70 @@
       <c r="BM7" s="6"/>
       <c r="BN7" s="6"/>
       <c r="CO7" s="1">
-        <f>SUM(CT7,CW7,CZ7,DC7,DF7,DI7,DL7,DO7,DR7)</f>
+        <f>SUM(CQ7,CS7,CU7,CW7,CY7,DA7,DC7,DE7,DG7)</f>
         <v>464.47498117251683</v>
       </c>
+      <c r="CP7">
+        <v>50</v>
+      </c>
+      <c r="CQ7">
+        <v>22.224677998651742</v>
+      </c>
+      <c r="CR7">
+        <v>150</v>
+      </c>
       <c r="CS7">
-        <v>50</v>
+        <v>29.769867310436624</v>
       </c>
       <c r="CT7">
-        <v>22.224677998651742</v>
+        <v>250</v>
+      </c>
+      <c r="CU7">
+        <v>34.148669739603761</v>
       </c>
       <c r="CV7">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="CW7">
-        <v>29.769867310436624</v>
+        <v>37.750023526841005</v>
+      </c>
+      <c r="CX7">
+        <v>450</v>
       </c>
       <c r="CY7">
-        <v>250</v>
+        <v>48.663972744195952</v>
       </c>
       <c r="CZ7">
-        <v>34.148669739603761</v>
+        <v>600</v>
+      </c>
+      <c r="DA7">
+        <v>69.211948417945436</v>
       </c>
       <c r="DB7">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="DC7">
-        <v>37.750023526841005</v>
+        <v>77.007212598030591</v>
+      </c>
+      <c r="DD7">
+        <v>1000</v>
       </c>
       <c r="DE7">
-        <v>450</v>
+        <v>73.265704602491368</v>
       </c>
       <c r="DF7">
-        <v>48.663972744195952</v>
-      </c>
-      <c r="DH7">
-        <v>600</v>
-      </c>
-      <c r="DI7">
-        <v>69.211948417945436</v>
-      </c>
-      <c r="DK7">
-        <v>800</v>
-      </c>
-      <c r="DL7">
-        <v>77.007212598030591</v>
-      </c>
-      <c r="DN7">
-        <v>1000</v>
-      </c>
-      <c r="DO7">
-        <v>73.265704602491368</v>
-      </c>
-      <c r="DQ7">
         <v>1200</v>
       </c>
-      <c r="DR7">
+      <c r="DG7">
         <v>72.432904234320333</v>
       </c>
     </row>
-    <row r="8" spans="1:166" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:152" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C8" s="7">
         <v>37602</v>
@@ -2138,7 +2035,7 @@
         <v>63</v>
       </c>
       <c r="H8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I8" s="6">
         <v>12</v>
@@ -2172,12 +2069,12 @@
       <c r="BM8" s="6"/>
       <c r="BN8" s="6"/>
     </row>
-    <row r="9" spans="1:166" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:152" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C9" s="7">
         <v>37606</v>
@@ -2186,7 +2083,7 @@
         <v>67</v>
       </c>
       <c r="H9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I9" s="6">
         <v>12</v>
@@ -2286,70 +2183,70 @@
       </c>
       <c r="CJ9" s="4"/>
       <c r="CO9" s="1">
-        <f>SUM(CT9,CW9,CZ9,DC9,DF9,DI9,DL9,DO9,DR9)</f>
+        <f>SUM(CQ9,CS9,CU9,CW9,CY9,DA9,DC9,DE9,DG9)</f>
         <v>488.5970080783672</v>
       </c>
+      <c r="CP9">
+        <v>50</v>
+      </c>
+      <c r="CQ9">
+        <v>26.139394561583618</v>
+      </c>
+      <c r="CR9">
+        <v>150</v>
+      </c>
       <c r="CS9">
-        <v>50</v>
+        <v>37.045159009435636</v>
       </c>
       <c r="CT9">
-        <v>26.139394561583618</v>
+        <v>250</v>
+      </c>
+      <c r="CU9">
+        <v>40.3124080742746</v>
       </c>
       <c r="CV9">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="CW9">
-        <v>37.045159009435636</v>
+        <v>39.950850841263758</v>
+      </c>
+      <c r="CX9">
+        <v>450</v>
       </c>
       <c r="CY9">
-        <v>250</v>
+        <v>50.045202623113795</v>
       </c>
       <c r="CZ9">
-        <v>40.3124080742746</v>
+        <v>600</v>
+      </c>
+      <c r="DA9">
+        <v>69.814459172113075</v>
       </c>
       <c r="DB9">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="DC9">
-        <v>39.950850841263758</v>
+        <v>77.8725124927644</v>
+      </c>
+      <c r="DD9">
+        <v>1000</v>
       </c>
       <c r="DE9">
-        <v>450</v>
+        <v>74.108661072713303</v>
       </c>
       <c r="DF9">
-        <v>50.045202623113795</v>
-      </c>
-      <c r="DH9">
-        <v>600</v>
-      </c>
-      <c r="DI9">
-        <v>69.814459172113075</v>
-      </c>
-      <c r="DK9">
-        <v>800</v>
-      </c>
-      <c r="DL9">
-        <v>77.8725124927644</v>
-      </c>
-      <c r="DN9">
-        <v>1000</v>
-      </c>
-      <c r="DO9">
-        <v>74.108661072713303</v>
-      </c>
-      <c r="DQ9">
         <v>1200</v>
       </c>
-      <c r="DR9">
+      <c r="DG9">
         <v>73.308360231105027</v>
       </c>
     </row>
-    <row r="10" spans="1:166" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:152" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C10" s="7">
         <v>37608</v>
@@ -2358,7 +2255,7 @@
         <v>69</v>
       </c>
       <c r="H10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I10" s="6">
         <v>12</v>
@@ -2414,12 +2311,12 @@
       <c r="CD10" s="4"/>
       <c r="CJ10" s="4"/>
     </row>
-    <row r="11" spans="1:166" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:152" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C11" s="7">
         <v>37613</v>
@@ -2428,7 +2325,7 @@
         <v>74</v>
       </c>
       <c r="H11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I11" s="6">
         <v>12</v>
@@ -2529,70 +2426,70 @@
       </c>
       <c r="CJ11" s="4"/>
       <c r="CO11" s="1">
-        <f>SUM(CT11,CW11,CZ11,DC11,DF11,DI11,DL11,DO11,DR11)</f>
+        <f>SUM(CQ11,CS11,CU11,CW11,CY11,DA11,DC11,DE11,DG11)</f>
         <v>479.46694964314531</v>
       </c>
+      <c r="CP11">
+        <v>50</v>
+      </c>
+      <c r="CQ11">
+        <v>25.889852149271359</v>
+      </c>
+      <c r="CR11">
+        <v>150</v>
+      </c>
       <c r="CS11">
-        <v>50</v>
+        <v>34.336252300286198</v>
       </c>
       <c r="CT11">
-        <v>25.889852149271359</v>
+        <v>250</v>
+      </c>
+      <c r="CU11">
+        <v>35.540055720572461</v>
       </c>
       <c r="CV11">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="CW11">
-        <v>34.336252300286198</v>
+        <v>37.911505549449778</v>
+      </c>
+      <c r="CX11">
+        <v>450</v>
       </c>
       <c r="CY11">
-        <v>250</v>
+        <v>48.55987269817458</v>
       </c>
       <c r="CZ11">
-        <v>35.540055720572461</v>
+        <v>600</v>
+      </c>
+      <c r="DA11">
+        <v>69.851782847150034</v>
       </c>
       <c r="DB11">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="DC11">
-        <v>37.911505549449778</v>
+        <v>77.344395186119343</v>
+      </c>
+      <c r="DD11">
+        <v>1000</v>
       </c>
       <c r="DE11">
-        <v>450</v>
+        <v>75.96722774802187</v>
       </c>
       <c r="DF11">
-        <v>48.55987269817458</v>
-      </c>
-      <c r="DH11">
-        <v>600</v>
-      </c>
-      <c r="DI11">
-        <v>69.851782847150034</v>
-      </c>
-      <c r="DK11">
-        <v>800</v>
-      </c>
-      <c r="DL11">
-        <v>77.344395186119343</v>
-      </c>
-      <c r="DN11">
-        <v>1000</v>
-      </c>
-      <c r="DO11">
-        <v>75.96722774802187</v>
-      </c>
-      <c r="DQ11">
         <v>1200</v>
       </c>
-      <c r="DR11">
+      <c r="DG11">
         <v>74.066005444099673</v>
       </c>
     </row>
-    <row r="12" spans="1:166" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:152" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C12" s="7">
         <v>37616</v>
@@ -2610,7 +2507,7 @@
         <v>77</v>
       </c>
       <c r="H12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I12" s="6">
         <v>12</v>
@@ -2662,12 +2559,12 @@
       <c r="CD12" s="4"/>
       <c r="CJ12" s="4"/>
     </row>
-    <row r="13" spans="1:166" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:152" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C13" s="7">
         <v>37620</v>
@@ -2676,7 +2573,7 @@
         <v>81</v>
       </c>
       <c r="H13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I13" s="6">
         <v>12</v>
@@ -2732,12 +2629,12 @@
       <c r="CD13" s="4"/>
       <c r="CJ13" s="4"/>
     </row>
-    <row r="14" spans="1:166" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:152" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C14" s="7">
         <v>37621</v>
@@ -2746,7 +2643,7 @@
         <v>82</v>
       </c>
       <c r="H14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I14" s="6">
         <v>12</v>
@@ -2795,70 +2692,70 @@
       <c r="CD14" s="4"/>
       <c r="CJ14" s="4"/>
       <c r="CO14" s="1">
-        <f>SUM(CT14,CW14,CZ14,DC14,DF14,DI14,DL14,DO14,DR14)</f>
+        <f>SUM(CQ14,CS14,CU14,CW14,CY14,DA14,DC14,DE14,DG14)</f>
         <v>429.33933270154881</v>
       </c>
+      <c r="CP14">
+        <v>50</v>
+      </c>
+      <c r="CQ14">
+        <v>22.78926371255157</v>
+      </c>
+      <c r="CR14">
+        <v>150</v>
+      </c>
       <c r="CS14">
-        <v>50</v>
+        <v>28.806845365134375</v>
       </c>
       <c r="CT14">
-        <v>22.78926371255157</v>
+        <v>250</v>
+      </c>
+      <c r="CU14">
+        <v>31.680669512270885</v>
       </c>
       <c r="CV14">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="CW14">
-        <v>28.806845365134375</v>
+        <v>33.322713527345144</v>
+      </c>
+      <c r="CX14">
+        <v>450</v>
       </c>
       <c r="CY14">
-        <v>250</v>
+        <v>43.685094248379471</v>
       </c>
       <c r="CZ14">
-        <v>31.680669512270885</v>
+        <v>600</v>
+      </c>
+      <c r="DA14">
+        <v>61.932641949020272</v>
       </c>
       <c r="DB14">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="DC14">
-        <v>33.322713527345144</v>
+        <v>70.779820321019926</v>
+      </c>
+      <c r="DD14">
+        <v>1000</v>
       </c>
       <c r="DE14">
-        <v>450</v>
+        <v>68.89920894804709</v>
       </c>
       <c r="DF14">
-        <v>43.685094248379471</v>
-      </c>
-      <c r="DH14">
-        <v>600</v>
-      </c>
-      <c r="DI14">
-        <v>61.932641949020272</v>
-      </c>
-      <c r="DK14">
-        <v>800</v>
-      </c>
-      <c r="DL14">
-        <v>70.779820321019926</v>
-      </c>
-      <c r="DN14">
-        <v>1000</v>
-      </c>
-      <c r="DO14">
-        <v>68.89920894804709</v>
-      </c>
-      <c r="DQ14">
         <v>1200</v>
       </c>
-      <c r="DR14">
+      <c r="DG14">
         <v>67.443075117780097</v>
       </c>
     </row>
-    <row r="15" spans="1:166" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:152" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C15" s="7">
         <v>37623</v>
@@ -2867,7 +2764,7 @@
         <v>84</v>
       </c>
       <c r="H15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I15" s="6">
         <v>12</v>
@@ -2965,12 +2862,12 @@
       </c>
       <c r="CJ15" s="4"/>
     </row>
-    <row r="16" spans="1:166" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:152" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C16" s="7">
         <v>37627</v>
@@ -2979,7 +2876,7 @@
         <v>88</v>
       </c>
       <c r="H16" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I16" s="6">
         <v>12</v>
@@ -3013,70 +2910,70 @@
       <c r="BM16" s="6"/>
       <c r="BN16" s="6"/>
       <c r="CO16" s="1">
-        <f>SUM(CT16,CW16,CZ16,DC16,DF16,DI16,DL16,DO16,DR16)</f>
+        <f>SUM(CQ16,CS16,CU16,CW16,CY16,DA16,DC16,DE16,DG16)</f>
         <v>485.76923713113706</v>
       </c>
+      <c r="CP16">
+        <v>50</v>
+      </c>
+      <c r="CQ16">
+        <v>26.437183970386467</v>
+      </c>
+      <c r="CR16">
+        <v>150</v>
+      </c>
       <c r="CS16">
-        <v>50</v>
+        <v>35.206376783247457</v>
       </c>
       <c r="CT16">
-        <v>26.437183970386467</v>
+        <v>250</v>
+      </c>
+      <c r="CU16">
+        <v>39.256173460984492</v>
       </c>
       <c r="CV16">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="CW16">
-        <v>35.206376783247457</v>
+        <v>39.966084994340058</v>
+      </c>
+      <c r="CX16">
+        <v>450</v>
       </c>
       <c r="CY16">
-        <v>250</v>
+        <v>49.61102926043926</v>
       </c>
       <c r="CZ16">
-        <v>39.256173460984492</v>
+        <v>600</v>
+      </c>
+      <c r="DA16">
+        <v>68.922245606944458</v>
       </c>
       <c r="DB16">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="DC16">
-        <v>39.966084994340058</v>
+        <v>76.82643398152517</v>
+      </c>
+      <c r="DD16">
+        <v>1000</v>
       </c>
       <c r="DE16">
-        <v>450</v>
+        <v>75.47567240875992</v>
       </c>
       <c r="DF16">
-        <v>49.61102926043926</v>
-      </c>
-      <c r="DH16">
-        <v>600</v>
-      </c>
-      <c r="DI16">
-        <v>68.922245606944458</v>
-      </c>
-      <c r="DK16">
-        <v>800</v>
-      </c>
-      <c r="DL16">
-        <v>76.82643398152517</v>
-      </c>
-      <c r="DN16">
-        <v>1000</v>
-      </c>
-      <c r="DO16">
-        <v>75.47567240875992</v>
-      </c>
-      <c r="DQ16">
         <v>1200</v>
       </c>
-      <c r="DR16">
+      <c r="DG16">
         <v>74.068036664509833</v>
       </c>
     </row>
-    <row r="17" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C17" s="7">
         <v>37628</v>
@@ -3085,7 +2982,7 @@
         <v>89</v>
       </c>
       <c r="H17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I17" s="6">
         <v>12</v>
@@ -3141,12 +3038,12 @@
       <c r="CD17" s="4"/>
       <c r="CJ17" s="4"/>
     </row>
-    <row r="18" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C18" s="7">
         <v>37631</v>
@@ -3155,7 +3052,7 @@
         <v>92</v>
       </c>
       <c r="H18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I18" s="6">
         <v>12</v>
@@ -3253,12 +3150,12 @@
       </c>
       <c r="CJ18" s="4"/>
     </row>
-    <row r="19" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C19" s="7">
         <v>37634</v>
@@ -3267,7 +3164,7 @@
         <v>95</v>
       </c>
       <c r="H19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I19" s="6">
         <v>12</v>
@@ -3301,70 +3198,70 @@
       <c r="BM19" s="6"/>
       <c r="BN19" s="6"/>
       <c r="CO19" s="1">
-        <f>SUM(CT19,CW19,CZ19,DC19,DF19,DI19,DL19,DO19,DR19)</f>
+        <f>SUM(CQ19,CS19,CU19,CW19,CY19,DA19,DC19,DE19,DG19)</f>
         <v>444.81396427018802</v>
       </c>
+      <c r="CP19">
+        <v>50</v>
+      </c>
+      <c r="CQ19">
+        <v>22.472942344831807</v>
+      </c>
+      <c r="CR19">
+        <v>150</v>
+      </c>
       <c r="CS19">
-        <v>50</v>
+        <v>27.726439082158251</v>
       </c>
       <c r="CT19">
-        <v>22.472942344831807</v>
+        <v>250</v>
+      </c>
+      <c r="CU19">
+        <v>28.17485051328411</v>
       </c>
       <c r="CV19">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="CW19">
-        <v>27.726439082158251</v>
+        <v>33.104622448774677</v>
+      </c>
+      <c r="CX19">
+        <v>450</v>
       </c>
       <c r="CY19">
-        <v>250</v>
+        <v>44.124195127458655</v>
       </c>
       <c r="CZ19">
-        <v>28.17485051328411</v>
+        <v>600</v>
+      </c>
+      <c r="DA19">
+        <v>64.429186059641154</v>
       </c>
       <c r="DB19">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="DC19">
-        <v>33.104622448774677</v>
+        <v>76.192693213551095</v>
+      </c>
+      <c r="DD19">
+        <v>1000</v>
       </c>
       <c r="DE19">
-        <v>450</v>
+        <v>75.073490767545607</v>
       </c>
       <c r="DF19">
-        <v>44.124195127458655</v>
-      </c>
-      <c r="DH19">
-        <v>600</v>
-      </c>
-      <c r="DI19">
-        <v>64.429186059641154</v>
-      </c>
-      <c r="DK19">
-        <v>800</v>
-      </c>
-      <c r="DL19">
-        <v>76.192693213551095</v>
-      </c>
-      <c r="DN19">
-        <v>1000</v>
-      </c>
-      <c r="DO19">
-        <v>75.073490767545607</v>
-      </c>
-      <c r="DQ19">
         <v>1200</v>
       </c>
-      <c r="DR19">
+      <c r="DG19">
         <v>73.515544712942699</v>
       </c>
     </row>
-    <row r="20" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C20" s="7">
         <v>37636</v>
@@ -3373,7 +3270,7 @@
         <v>97</v>
       </c>
       <c r="H20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I20" s="6">
         <v>12</v>
@@ -3429,12 +3326,12 @@
       <c r="CD20" s="4"/>
       <c r="CJ20" s="4"/>
     </row>
-    <row r="21" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C21" s="7">
         <v>37641</v>
@@ -3443,7 +3340,7 @@
         <v>102</v>
       </c>
       <c r="H21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I21" s="6">
         <v>12</v>
@@ -3477,12 +3374,12 @@
       <c r="BM21" s="6"/>
       <c r="BN21" s="6"/>
     </row>
-    <row r="22" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C22" s="7">
         <v>37642</v>
@@ -3491,7 +3388,7 @@
         <v>103</v>
       </c>
       <c r="H22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I22" s="6">
         <v>12</v>
@@ -3596,12 +3493,12 @@
       </c>
       <c r="CJ22" s="4"/>
     </row>
-    <row r="23" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C23" s="7">
         <v>37645</v>
@@ -3610,7 +3507,7 @@
         <v>106</v>
       </c>
       <c r="H23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I23" s="6">
         <v>12</v>
@@ -3662,70 +3559,70 @@
       <c r="CD23" s="1"/>
       <c r="CJ23" s="4"/>
       <c r="CO23" s="1">
-        <f>SUM(CT23,CW23,CZ23,DC23,DF23,DI23,DL23,DO23,DR23)</f>
+        <f>SUM(CQ23,CS23,CU23,CW23,CY23,DA23,DC23,DE23,DG23)</f>
         <v>457.97255101038525</v>
       </c>
+      <c r="CP23">
+        <v>50</v>
+      </c>
+      <c r="CQ23">
+        <v>23.034971926467222</v>
+      </c>
+      <c r="CR23">
+        <v>150</v>
+      </c>
       <c r="CS23">
-        <v>50</v>
+        <v>30.860302057376469</v>
       </c>
       <c r="CT23">
-        <v>23.034971926467222</v>
+        <v>250</v>
+      </c>
+      <c r="CU23">
+        <v>33.575865583934892</v>
       </c>
       <c r="CV23">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="CW23">
-        <v>30.860302057376469</v>
+        <v>36.649102064527078</v>
+      </c>
+      <c r="CX23">
+        <v>450</v>
       </c>
       <c r="CY23">
-        <v>250</v>
+        <v>46.684802357033362</v>
       </c>
       <c r="CZ23">
-        <v>33.575865583934892</v>
+        <v>600</v>
+      </c>
+      <c r="DA23">
+        <v>65.069020488845737</v>
       </c>
       <c r="DB23">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="DC23">
-        <v>36.649102064527078</v>
+        <v>73.844602419390768</v>
+      </c>
+      <c r="DD23">
+        <v>1000</v>
       </c>
       <c r="DE23">
-        <v>450</v>
+        <v>73.889289268414586</v>
       </c>
       <c r="DF23">
-        <v>46.684802357033362</v>
-      </c>
-      <c r="DH23">
-        <v>600</v>
-      </c>
-      <c r="DI23">
-        <v>65.069020488845737</v>
-      </c>
-      <c r="DK23">
-        <v>800</v>
-      </c>
-      <c r="DL23">
-        <v>73.844602419390768</v>
-      </c>
-      <c r="DN23">
-        <v>1000</v>
-      </c>
-      <c r="DO23">
-        <v>73.889289268414586</v>
-      </c>
-      <c r="DQ23">
         <v>1200</v>
       </c>
-      <c r="DR23">
+      <c r="DG23">
         <v>74.364594844395143</v>
       </c>
     </row>
-    <row r="24" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C24" s="7">
         <v>37650</v>
@@ -3734,7 +3631,7 @@
         <v>111</v>
       </c>
       <c r="H24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I24" s="6">
         <v>12</v>
@@ -3790,12 +3687,12 @@
       <c r="CD24" s="4"/>
       <c r="CJ24" s="4"/>
     </row>
-    <row r="25" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C25" s="7">
         <v>37652</v>
@@ -3804,7 +3701,7 @@
         <v>113</v>
       </c>
       <c r="H25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I25" s="6">
         <v>12</v>
@@ -3902,12 +3799,12 @@
       </c>
       <c r="CJ25" s="4"/>
     </row>
-    <row r="26" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C26" s="7">
         <v>37655</v>
@@ -3916,7 +3813,7 @@
         <v>116</v>
       </c>
       <c r="H26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I26" s="6">
         <v>12</v>
@@ -3950,70 +3847,70 @@
       <c r="BM26" s="6"/>
       <c r="BN26" s="6"/>
       <c r="CO26" s="1">
-        <f>SUM(CT26,CW26,CZ26,DC26,DF26,DI26,DL26,DO26,DR26)</f>
+        <f>SUM(CQ26,CS26,CU26,CW26,CY26,DA26,DC26,DE26,DG26)</f>
         <v>474.36010481440292</v>
       </c>
+      <c r="CP26">
+        <v>50</v>
+      </c>
+      <c r="CQ26">
+        <v>24.514972507556063</v>
+      </c>
+      <c r="CR26">
+        <v>150</v>
+      </c>
       <c r="CS26">
-        <v>50</v>
+        <v>33.333739539429544</v>
       </c>
       <c r="CT26">
-        <v>24.514972507556063</v>
+        <v>250</v>
+      </c>
+      <c r="CU26">
+        <v>37.44026241428957</v>
       </c>
       <c r="CV26">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="CW26">
-        <v>33.333739539429544</v>
+        <v>38.888522566743127</v>
+      </c>
+      <c r="CX26">
+        <v>450</v>
       </c>
       <c r="CY26">
-        <v>250</v>
+        <v>48.983889958798244</v>
       </c>
       <c r="CZ26">
-        <v>37.44026241428957</v>
+        <v>600</v>
+      </c>
+      <c r="DA26">
+        <v>67.519941816271071</v>
       </c>
       <c r="DB26">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="DC26">
-        <v>38.888522566743127</v>
+        <v>75.569108547627891</v>
+      </c>
+      <c r="DD26">
+        <v>1000</v>
       </c>
       <c r="DE26">
-        <v>450</v>
+        <v>73.992881509333429</v>
       </c>
       <c r="DF26">
-        <v>48.983889958798244</v>
-      </c>
-      <c r="DH26">
-        <v>600</v>
-      </c>
-      <c r="DI26">
-        <v>67.519941816271071</v>
-      </c>
-      <c r="DK26">
-        <v>800</v>
-      </c>
-      <c r="DL26">
-        <v>75.569108547627891</v>
-      </c>
-      <c r="DN26">
-        <v>1000</v>
-      </c>
-      <c r="DO26">
-        <v>73.992881509333429</v>
-      </c>
-      <c r="DQ26">
         <v>1200</v>
       </c>
-      <c r="DR26">
+      <c r="DG26">
         <v>74.116785954353986</v>
       </c>
     </row>
-    <row r="27" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C27" s="7">
         <v>37657</v>
@@ -4022,7 +3919,7 @@
         <v>118</v>
       </c>
       <c r="H27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I27" s="6">
         <v>12</v>
@@ -4079,12 +3976,12 @@
       <c r="CD27" s="4"/>
       <c r="CJ27" s="4"/>
     </row>
-    <row r="28" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B28" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C28" s="7">
         <v>37662</v>
@@ -4093,7 +3990,7 @@
         <v>123</v>
       </c>
       <c r="H28" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I28" s="6">
         <v>12</v>
@@ -4189,70 +4086,70 @@
       </c>
       <c r="CJ28" s="4"/>
       <c r="CO28" s="1">
-        <f>SUM(CT28,CW28,CZ28,DC28,DF28,DI28,DL28,DO28,DR28)</f>
+        <f>SUM(CQ28,CS28,CU28,CW28,CY28,DA28,DC28,DE28,DG28)</f>
         <v>434.6434252804865</v>
       </c>
+      <c r="CP28">
+        <v>50</v>
+      </c>
+      <c r="CQ28">
+        <v>22.757951092312641</v>
+      </c>
+      <c r="CR28">
+        <v>150</v>
+      </c>
       <c r="CS28">
-        <v>50</v>
+        <v>29.639500227623611</v>
       </c>
       <c r="CT28">
-        <v>22.757951092312641</v>
+        <v>250</v>
+      </c>
+      <c r="CU28">
+        <v>31.268399197978027</v>
       </c>
       <c r="CV28">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="CW28">
-        <v>29.639500227623611</v>
+        <v>33.986172106789894</v>
+      </c>
+      <c r="CX28">
+        <v>450</v>
       </c>
       <c r="CY28">
-        <v>250</v>
+        <v>43.57576561671187</v>
       </c>
       <c r="CZ28">
-        <v>31.268399197978027</v>
+        <v>600</v>
+      </c>
+      <c r="DA28">
+        <v>60.053429491025334</v>
       </c>
       <c r="DB28">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="DC28">
-        <v>33.986172106789894</v>
+        <v>69.382011178240035</v>
+      </c>
+      <c r="DD28">
+        <v>1000</v>
       </c>
       <c r="DE28">
-        <v>450</v>
+        <v>71.149172935090817</v>
       </c>
       <c r="DF28">
-        <v>43.57576561671187</v>
-      </c>
-      <c r="DH28">
-        <v>600</v>
-      </c>
-      <c r="DI28">
-        <v>60.053429491025334</v>
-      </c>
-      <c r="DK28">
-        <v>800</v>
-      </c>
-      <c r="DL28">
-        <v>69.382011178240035</v>
-      </c>
-      <c r="DN28">
-        <v>1000</v>
-      </c>
-      <c r="DO28">
-        <v>71.149172935090817</v>
-      </c>
-      <c r="DQ28">
         <v>1200</v>
       </c>
-      <c r="DR28">
+      <c r="DG28">
         <v>72.831023434714282</v>
       </c>
     </row>
-    <row r="29" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C29" s="7">
         <v>37663</v>
@@ -4261,7 +4158,7 @@
         <v>124</v>
       </c>
       <c r="H29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I29" s="6">
         <v>12</v>
@@ -4295,24 +4192,24 @@
       <c r="BM29" s="6"/>
       <c r="BN29" s="6"/>
     </row>
-    <row r="30" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C30" s="7">
         <v>37669</v>
       </c>
       <c r="E30" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G30">
         <v>130</v>
       </c>
       <c r="H30" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I30" s="6">
         <v>12</v>
@@ -4347,12 +4244,12 @@
         <v>7.5645800506135688</v>
       </c>
     </row>
-    <row r="31" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C31" s="7">
         <v>37670</v>
@@ -4361,7 +4258,7 @@
         <v>131</v>
       </c>
       <c r="H31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I31" s="6">
         <v>12</v>
@@ -4394,82 +4291,82 @@
       <c r="BN31" s="6"/>
       <c r="CJ31" s="1"/>
       <c r="CO31" s="1">
-        <f>SUM(CT31,CW31,CZ31,DC31,DF31,DI31,DL31,DO31,DR31)</f>
+        <f>SUM(CQ31,CS31,CU31,CW31,CY31,DA31,DC31,DE31,DG31)</f>
         <v>476.79207601374992</v>
       </c>
+      <c r="CP31">
+        <v>50</v>
+      </c>
+      <c r="CQ31">
+        <v>24.406975919385072</v>
+      </c>
+      <c r="CR31">
+        <v>150</v>
+      </c>
       <c r="CS31">
-        <v>50</v>
+        <v>33.809225682557617</v>
       </c>
       <c r="CT31">
-        <v>24.406975919385072</v>
+        <v>250</v>
+      </c>
+      <c r="CU31">
+        <v>38.026269502624565</v>
       </c>
       <c r="CV31">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="CW31">
-        <v>33.809225682557617</v>
+        <v>39.718276104298916</v>
+      </c>
+      <c r="CX31">
+        <v>450</v>
       </c>
       <c r="CY31">
-        <v>250</v>
+        <v>48.870903323482366</v>
       </c>
       <c r="CZ31">
-        <v>38.026269502624565</v>
+        <v>600</v>
+      </c>
+      <c r="DA31">
+        <v>68.230868959831739</v>
       </c>
       <c r="DB31">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="DC31">
-        <v>39.718276104298916</v>
+        <v>76.030195580737228</v>
+      </c>
+      <c r="DD31">
+        <v>1000</v>
       </c>
       <c r="DE31">
-        <v>450</v>
+        <v>74.384907048496871</v>
       </c>
       <c r="DF31">
-        <v>48.870903323482366</v>
-      </c>
-      <c r="DH31">
-        <v>600</v>
-      </c>
-      <c r="DI31">
-        <v>68.230868959831739</v>
-      </c>
-      <c r="DK31">
-        <v>800</v>
-      </c>
-      <c r="DL31">
-        <v>76.030195580737228</v>
-      </c>
-      <c r="DN31">
-        <v>1000</v>
-      </c>
-      <c r="DO31">
-        <v>74.384907048496871</v>
-      </c>
-      <c r="DQ31">
         <v>1200</v>
       </c>
-      <c r="DR31">
+      <c r="DG31">
         <v>73.31445389233555</v>
       </c>
     </row>
-    <row r="32" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C32" s="7">
         <v>37677</v>
       </c>
       <c r="E32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G32">
         <v>138</v>
       </c>
       <c r="H32" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I32" s="6">
         <v>12</v>
@@ -4570,12 +4467,12 @@
         <v>22.162536408346469</v>
       </c>
     </row>
-    <row r="33" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C33" s="7">
         <v>37678</v>
@@ -4584,7 +4481,7 @@
         <v>139</v>
       </c>
       <c r="H33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I33" s="6">
         <v>12</v>
@@ -4636,82 +4533,82 @@
       <c r="CD33" s="1"/>
       <c r="CJ33" s="1"/>
       <c r="CO33" s="1">
-        <f>SUM(CT33,CW33,CZ33,DC33,DF33,DI33,DL33,DO33,DR33)</f>
+        <f>SUM(CQ33,CS33,CU33,CW33,CY33,DA33,DC33,DE33,DG33)</f>
         <v>475.3926194563083</v>
       </c>
+      <c r="CP33">
+        <v>50</v>
+      </c>
+      <c r="CQ33">
+        <v>24.007899769605288</v>
+      </c>
+      <c r="CR33">
+        <v>150</v>
+      </c>
       <c r="CS33">
-        <v>50</v>
+        <v>34.526749936799781</v>
       </c>
       <c r="CT33">
-        <v>24.007899769605288</v>
+        <v>250</v>
+      </c>
+      <c r="CU33">
+        <v>39.182033916013175</v>
       </c>
       <c r="CV33">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="CW33">
-        <v>34.526749936799781</v>
+        <v>40.413969094783262</v>
+      </c>
+      <c r="CX33">
+        <v>450</v>
       </c>
       <c r="CY33">
-        <v>250</v>
+        <v>50.598710184886016</v>
       </c>
       <c r="CZ33">
-        <v>39.182033916013175</v>
+        <v>600</v>
+      </c>
+      <c r="DA33">
+        <v>68.470806870783449</v>
       </c>
       <c r="DB33">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="DC33">
-        <v>40.413969094783262</v>
+        <v>73.588668647708943</v>
+      </c>
+      <c r="DD33">
+        <v>1000</v>
       </c>
       <c r="DE33">
-        <v>450</v>
+        <v>72.168845580997811</v>
       </c>
       <c r="DF33">
-        <v>50.598710184886016</v>
-      </c>
-      <c r="DH33">
-        <v>600</v>
-      </c>
-      <c r="DI33">
-        <v>68.470806870783449</v>
-      </c>
-      <c r="DK33">
-        <v>800</v>
-      </c>
-      <c r="DL33">
-        <v>73.588668647708943</v>
-      </c>
-      <c r="DN33">
-        <v>1000</v>
-      </c>
-      <c r="DO33">
-        <v>72.168845580997811</v>
-      </c>
-      <c r="DQ33">
         <v>1200</v>
       </c>
-      <c r="DR33">
+      <c r="DG33">
         <v>72.434935454730507</v>
       </c>
     </row>
-    <row r="34" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C34" s="7">
         <v>37683</v>
       </c>
       <c r="E34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G34">
         <v>144</v>
       </c>
       <c r="H34" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I34" s="6">
         <v>12</v>
@@ -4746,70 +4643,70 @@
         <v>46.083416893472759</v>
       </c>
       <c r="CO34" s="1">
-        <f>SUM(CT34,CW34,CZ34,DC34,DF34,DI34,DL34,DO34,DR34)</f>
+        <f>SUM(CQ34,CS34,CU34,CW34,CY34,DA34,DC34,DE34,DG34)</f>
         <v>461.88263957792879</v>
       </c>
+      <c r="CP34">
+        <v>50</v>
+      </c>
+      <c r="CQ34">
+        <v>23.872424759591976</v>
+      </c>
+      <c r="CR34">
+        <v>150</v>
+      </c>
       <c r="CS34">
-        <v>50</v>
+        <v>33.387301209112401</v>
       </c>
       <c r="CT34">
-        <v>23.872424759591976</v>
+        <v>250</v>
+      </c>
+      <c r="CU34">
+        <v>36.696835744166144</v>
       </c>
       <c r="CV34">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="CW34">
-        <v>33.387301209112401</v>
+        <v>38.771727393158159</v>
+      </c>
+      <c r="CX34">
+        <v>450</v>
       </c>
       <c r="CY34">
-        <v>250</v>
+        <v>48.253920123892236</v>
       </c>
       <c r="CZ34">
-        <v>36.696835744166144</v>
+        <v>600</v>
+      </c>
+      <c r="DA34">
+        <v>65.728405414498255</v>
       </c>
       <c r="DB34">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="DC34">
-        <v>38.771727393158159</v>
+        <v>72.004316727773769</v>
+      </c>
+      <c r="DD34">
+        <v>1000</v>
       </c>
       <c r="DE34">
-        <v>450</v>
+        <v>71.939317674648223</v>
       </c>
       <c r="DF34">
-        <v>48.253920123892236</v>
-      </c>
-      <c r="DH34">
-        <v>600</v>
-      </c>
-      <c r="DI34">
-        <v>65.728405414498255</v>
-      </c>
-      <c r="DK34">
-        <v>800</v>
-      </c>
-      <c r="DL34">
-        <v>72.004316727773769</v>
-      </c>
-      <c r="DN34">
-        <v>1000</v>
-      </c>
-      <c r="DO34">
-        <v>71.939317674648223</v>
-      </c>
-      <c r="DQ34">
         <v>1200</v>
       </c>
-      <c r="DR34">
+      <c r="DG34">
         <v>71.22839053108757</v>
       </c>
     </row>
-    <row r="35" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B35" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C35" s="7">
         <v>37687</v>
@@ -4827,7 +4724,7 @@
         <v>148</v>
       </c>
       <c r="H35" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I35" s="6">
         <v>12</v>
@@ -4880,12 +4777,12 @@
       <c r="CD35" s="4"/>
       <c r="CJ35" s="4"/>
     </row>
-    <row r="36" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B36" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C36" s="7">
         <v>37690</v>
@@ -4894,7 +4791,7 @@
         <v>151</v>
       </c>
       <c r="H36" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I36" s="6">
         <v>12</v>
@@ -4928,82 +4825,82 @@
       <c r="BM36" s="6"/>
       <c r="BN36" s="6"/>
       <c r="CO36" s="1">
-        <f>SUM(CT36,CW36,CZ36,DC36,DF36,DI36,DL36,DO36,DR36)</f>
+        <f>SUM(CQ36,CS36,CU36,CW36,CY36,DA36,DC36,DE36,DG36)</f>
         <v>439.48360294283111</v>
       </c>
+      <c r="CP36">
+        <v>50</v>
+      </c>
+      <c r="CQ36">
+        <v>22.438115042729322</v>
+      </c>
+      <c r="CR36">
+        <v>150</v>
+      </c>
       <c r="CS36">
-        <v>50</v>
+        <v>29.802711730525171</v>
       </c>
       <c r="CT36">
-        <v>22.438115042729322</v>
+        <v>250</v>
+      </c>
+      <c r="CU36">
+        <v>32.344946015369871</v>
       </c>
       <c r="CV36">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="CW36">
-        <v>29.802711730525171</v>
+        <v>35.594898671647144</v>
+      </c>
+      <c r="CX36">
+        <v>450</v>
       </c>
       <c r="CY36">
-        <v>250</v>
+        <v>45.570170156950759</v>
       </c>
       <c r="CZ36">
-        <v>32.344946015369871</v>
+        <v>600</v>
+      </c>
+      <c r="DA36">
+        <v>62.810049490181768</v>
       </c>
       <c r="DB36">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="DC36">
-        <v>35.594898671647144</v>
+        <v>69.587164439667561</v>
+      </c>
+      <c r="DD36">
+        <v>1000</v>
       </c>
       <c r="DE36">
-        <v>450</v>
+        <v>69.956846554319085</v>
       </c>
       <c r="DF36">
-        <v>45.570170156950759</v>
-      </c>
-      <c r="DH36">
-        <v>600</v>
-      </c>
-      <c r="DI36">
-        <v>62.810049490181768</v>
-      </c>
-      <c r="DK36">
-        <v>800</v>
-      </c>
-      <c r="DL36">
-        <v>69.587164439667561</v>
-      </c>
-      <c r="DN36">
-        <v>1000</v>
-      </c>
-      <c r="DO36">
-        <v>69.956846554319085</v>
-      </c>
-      <c r="DQ36">
         <v>1200</v>
       </c>
-      <c r="DR36">
+      <c r="DG36">
         <v>71.378700841440391</v>
       </c>
     </row>
-    <row r="37" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B37" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C37" s="7">
         <v>37692</v>
       </c>
       <c r="E37" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G37">
         <v>153</v>
       </c>
       <c r="H37" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I37" s="6">
         <v>12</v>
@@ -5038,12 +4935,12 @@
         <v>73.285823425488232</v>
       </c>
     </row>
-    <row r="38" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B38" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C38" s="7">
         <v>37697</v>
@@ -5052,7 +4949,7 @@
         <v>158</v>
       </c>
       <c r="H38" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I38" s="6">
         <v>12</v>
@@ -5136,12 +5033,12 @@
         <v>96.67</v>
       </c>
     </row>
-    <row r="39" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B39" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C39" s="7">
         <v>37698</v>
@@ -5150,7 +5047,7 @@
         <v>159</v>
       </c>
       <c r="H39" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I39" s="6">
         <v>12</v>
@@ -5192,82 +5089,82 @@
       <c r="CC39" s="1"/>
       <c r="CD39" s="1"/>
       <c r="CO39" s="1">
-        <f>SUM(CT39,CW39,CZ39,DC39,DF39,DI39,DL39,DO39,DR39)</f>
+        <f>SUM(CQ39,CS39,CU39,CW39,CY39,DA39,DC39,DE39,DG39)</f>
         <v>400.38249029362578</v>
       </c>
+      <c r="CP39">
+        <v>50</v>
+      </c>
+      <c r="CQ39">
+        <v>21.40256195911341</v>
+      </c>
+      <c r="CR39">
+        <v>150</v>
+      </c>
       <c r="CS39">
-        <v>50</v>
+        <v>26.010949755994783</v>
       </c>
       <c r="CT39">
-        <v>21.40256195911341</v>
+        <v>250</v>
+      </c>
+      <c r="CU39">
+        <v>24.886304669213555</v>
       </c>
       <c r="CV39">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="CW39">
-        <v>26.010949755994783</v>
+        <v>29.524596475844262</v>
+      </c>
+      <c r="CX39">
+        <v>450</v>
       </c>
       <c r="CY39">
-        <v>250</v>
+        <v>39.360983265602293</v>
       </c>
       <c r="CZ39">
-        <v>24.886304669213555</v>
+        <v>600</v>
+      </c>
+      <c r="DA39">
+        <v>56.129111658570544</v>
       </c>
       <c r="DB39">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="DC39">
-        <v>29.524596475844262</v>
+        <v>65.989873093250665</v>
+      </c>
+      <c r="DD39">
+        <v>1000</v>
       </c>
       <c r="DE39">
-        <v>450</v>
+        <v>67.478757653907678</v>
       </c>
       <c r="DF39">
-        <v>39.360983265602293</v>
-      </c>
-      <c r="DH39">
-        <v>600</v>
-      </c>
-      <c r="DI39">
-        <v>56.129111658570544</v>
-      </c>
-      <c r="DK39">
-        <v>800</v>
-      </c>
-      <c r="DL39">
-        <v>65.989873093250665</v>
-      </c>
-      <c r="DN39">
-        <v>1000</v>
-      </c>
-      <c r="DO39">
-        <v>67.478757653907678</v>
-      </c>
-      <c r="DQ39">
         <v>1200</v>
       </c>
-      <c r="DR39">
+      <c r="DG39">
         <v>69.599351762128592</v>
       </c>
     </row>
-    <row r="40" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B40" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C40" s="7">
         <v>37699</v>
       </c>
       <c r="E40" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G40">
         <v>160</v>
       </c>
       <c r="H40" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I40" s="6">
         <v>12</v>
@@ -5304,24 +5201,24 @@
         <v>92.72549300482261</v>
       </c>
     </row>
-    <row r="41" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B41" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C41" s="7">
         <v>37708</v>
       </c>
       <c r="E41" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G41">
         <v>169</v>
       </c>
       <c r="H41" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I41" s="6">
         <v>12</v>
@@ -5355,12 +5252,12 @@
         <v>97.945614286396406</v>
       </c>
     </row>
-    <row r="42" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C42" s="7">
         <v>37712</v>
@@ -5369,7 +5266,7 @@
         <v>173</v>
       </c>
       <c r="H42" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I42" s="6">
         <v>12</v>
@@ -5452,24 +5349,24 @@
         <v>127.08</v>
       </c>
     </row>
-    <row r="43" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C43" s="7">
         <v>37718</v>
       </c>
       <c r="E43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G43">
         <v>179</v>
       </c>
       <c r="H43" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I43" s="6">
         <v>12</v>
@@ -5496,12 +5393,12 @@
         <v>99.358974358974365</v>
       </c>
     </row>
-    <row r="44" spans="1:122" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:111" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="B44" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C44" s="7">
         <v>37722</v>
@@ -5519,7 +5416,7 @@
         <v>183</v>
       </c>
       <c r="H44" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I44" s="6">
         <v>12</v>
@@ -5568,12 +5465,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:FJ44" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:FJ11">
+  <autoFilter ref="A1:EV44" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:EV11">
       <sortCondition ref="A1:A41"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:FJ44">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:EV44">
     <sortCondition ref="A2:A44"/>
     <sortCondition ref="G2:G44"/>
   </sortState>

</xml_diff>

<commit_message>
Added extra datasets for DD and Narrabri and fitting of soil parameters
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/Narrabri0203Observed.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/Narrabri0203Observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43ED442-5FD9-4869-A25A-0A55976329FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BD2DBE-D23D-4B78-A261-94B0C3B406EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
@@ -506,34 +506,34 @@
     <t>Narrabri0203RowSpacing1m</t>
   </si>
   <si>
-    <t>Soil.Water.PAWmm(1)</t>
-  </si>
-  <si>
-    <t>Soil.Water.PAWmm(2)</t>
-  </si>
-  <si>
-    <t>Soil.Water.PAWmm(3)</t>
-  </si>
-  <si>
-    <t>Soil.Water.PAWmm(4)</t>
-  </si>
-  <si>
-    <t>Soil.Water.PAWmm(5)</t>
-  </si>
-  <si>
-    <t>Soil.Water.PAWmm(6)</t>
-  </si>
-  <si>
-    <t>Soil.Water.PAWmm(7)</t>
-  </si>
-  <si>
-    <t>Soil.Water.PAWmm(8)</t>
-  </si>
-  <si>
-    <t>Soil.Water.PAWmm(9)</t>
-  </si>
-  <si>
-    <t>TotalPAWmm</t>
+    <t>Soil.Water.MM(1)</t>
+  </si>
+  <si>
+    <t>Soil.Water.MM(2)</t>
+  </si>
+  <si>
+    <t>Soil.Water.MM(3)</t>
+  </si>
+  <si>
+    <t>Soil.Water.MM(4)</t>
+  </si>
+  <si>
+    <t>Soil.Water.MM(5)</t>
+  </si>
+  <si>
+    <t>Soil.Water.MM(6)</t>
+  </si>
+  <si>
+    <t>Soil.Water.MM(7)</t>
+  </si>
+  <si>
+    <t>Soil.Water.MM(8)</t>
+  </si>
+  <si>
+    <t>Soil.Water.MM(9)</t>
+  </si>
+  <si>
+    <t>TotalSWmm</t>
   </si>
 </sst>
 </file>
@@ -932,7 +932,7 @@
   <dimension ref="A1:EV44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="CN2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="CK2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="CO2" sqref="CO2"/>

</xml_diff>

<commit_message>
Added UNR treatment to Narrabri0203
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/Narrabri0203Observed.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/Narrabri0203Observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C0E799-CD46-47D7-A689-61FCC7A4339F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8096058-C834-40DB-B4F1-36783EEA8159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="17640" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="166">
   <si>
     <t>SimulationName</t>
   </si>
@@ -491,9 +491,6 @@
     <t>Soil.Water.MM(12)</t>
   </si>
   <si>
-    <t>Narrabri0203RowSpacing1m</t>
-  </si>
-  <si>
     <t>Soil.Water.MM(1)</t>
   </si>
   <si>
@@ -528,6 +525,15 @@
   </si>
   <si>
     <t>Cotton.Leaf.SpecificAreaCanopy</t>
+  </si>
+  <si>
+    <t>Narrabri0203UNR</t>
+  </si>
+  <si>
+    <t>EXP 2: 2002-2003 Narrabri growth analysis: UNR (0.38m) treatment</t>
+  </si>
+  <si>
+    <t>Narrabri0203Conventional</t>
   </si>
 </sst>
 </file>
@@ -539,7 +545,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -558,6 +564,17 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -591,11 +608,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -608,10 +626,19 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{4980968D-DE36-44C4-8BE9-28B36F352809}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -923,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:ET44"/>
+  <dimension ref="A1:ET75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
@@ -934,14 +961,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.140625" customWidth="1"/>
     <col min="5" max="5" width="37.5703125" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
     <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.140625" customWidth="1"/>
     <col min="10" max="10" width="32" customWidth="1"/>
     <col min="11" max="11" width="19.140625" customWidth="1"/>
@@ -975,31 +1002,32 @@
     <col min="40" max="40" width="29.5703125" customWidth="1"/>
     <col min="41" max="41" width="26.28515625" customWidth="1"/>
     <col min="42" max="42" width="24" customWidth="1"/>
-    <col min="43" max="43" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="48" width="12" style="11" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12" style="11" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="7.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="12" style="11" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="12" style="11" customWidth="1"/>
     <col min="53" max="53" width="7.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="10.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="10" style="11" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="12.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="7.7109375" style="11" customWidth="1"/>
+    <col min="56" max="56" width="8.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="26.7109375" customWidth="1"/>
-    <col min="67" max="67" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="6.7109375" bestFit="1" customWidth="1"/>
@@ -1022,31 +1050,31 @@
     <col min="88" max="88" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="12" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="14" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="12" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="12" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="12" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="100" max="100" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="12" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="12" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="104" max="104" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="12" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="106" max="106" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="12" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="108" max="108" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="12" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="110" max="110" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="13" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="112" max="112" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="13" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="114" max="114" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="13" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="116" max="116" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="117" max="117" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="118" max="118" width="18.28515625" bestFit="1" customWidth="1"/>
@@ -1198,7 +1226,7 @@
         <v>130</v>
       </c>
       <c r="AQ1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AR1" t="s">
         <v>58</v>
@@ -1249,7 +1277,7 @@
         <v>102</v>
       </c>
       <c r="BH1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="BI1" t="s">
         <v>103</v>
@@ -1342,61 +1370,61 @@
         <v>66</v>
       </c>
       <c r="CM1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="CN1" t="s">
         <v>78</v>
       </c>
       <c r="CO1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="CP1" t="s">
         <v>79</v>
       </c>
       <c r="CQ1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="CR1" t="s">
         <v>87</v>
       </c>
       <c r="CS1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="CT1" t="s">
         <v>86</v>
       </c>
       <c r="CU1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="CV1" t="s">
         <v>85</v>
       </c>
       <c r="CW1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="CX1" t="s">
         <v>92</v>
       </c>
       <c r="CY1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="CZ1" t="s">
         <v>93</v>
       </c>
       <c r="DA1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="DB1" t="s">
         <v>84</v>
       </c>
       <c r="DC1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="DD1" t="s">
         <v>83</v>
       </c>
       <c r="DE1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="DF1" t="s">
         <v>82</v>
@@ -1524,7 +1552,7 @@
     </row>
     <row r="2" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
         <v>122</v>
@@ -1541,12 +1569,14 @@
       <c r="H2" t="s">
         <v>124</v>
       </c>
-      <c r="I2" s="6">
-        <v>12</v>
+      <c r="I2">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J2">
         <v>1000</v>
       </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
       <c r="R2">
         <v>53</v>
       </c>
@@ -1612,7 +1642,7 @@
     </row>
     <row r="3" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
         <v>122</v>
@@ -1635,14 +1665,14 @@
       <c r="H3" t="s">
         <v>124</v>
       </c>
-      <c r="I3" s="6">
-        <v>12</v>
+      <c r="I3">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J3">
         <v>1000</v>
       </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="R3">
@@ -1693,7 +1723,7 @@
     </row>
     <row r="4" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
         <v>122</v>
@@ -1716,14 +1746,14 @@
       <c r="H4" t="s">
         <v>124</v>
       </c>
-      <c r="I4" s="6">
-        <v>12</v>
+      <c r="I4">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J4">
         <v>1000</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="R4">
@@ -1774,7 +1804,7 @@
     </row>
     <row r="5" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
         <v>122</v>
@@ -1788,14 +1818,14 @@
       <c r="H5" t="s">
         <v>124</v>
       </c>
-      <c r="I5" s="6">
-        <v>12</v>
+      <c r="I5">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J5">
         <v>1000</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="R5">
@@ -1894,7 +1924,7 @@
     </row>
     <row r="6" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s">
         <v>122</v>
@@ -1908,12 +1938,14 @@
       <c r="H6" t="s">
         <v>124</v>
       </c>
-      <c r="I6" s="6">
-        <v>12</v>
+      <c r="I6">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J6">
         <v>1000</v>
       </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
       <c r="P6" s="4">
         <v>0.22240889723649346</v>
       </c>
@@ -1955,7 +1987,7 @@
     </row>
     <row r="7" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
         <v>122</v>
@@ -1969,12 +2001,14 @@
       <c r="H7" t="s">
         <v>124</v>
       </c>
-      <c r="I7" s="6">
-        <v>12</v>
+      <c r="I7">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J7">
         <v>1000</v>
       </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
       <c r="P7" s="4"/>
       <c r="R7">
         <v>53</v>
@@ -2072,7 +2106,7 @@
     </row>
     <row r="8" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
         <v>122</v>
@@ -2086,12 +2120,14 @@
       <c r="H8" t="s">
         <v>124</v>
       </c>
-      <c r="I8" s="6">
-        <v>12</v>
+      <c r="I8">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J8">
         <v>1000</v>
       </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
       <c r="P8" s="4">
         <v>0.33731543685906962</v>
       </c>
@@ -2132,7 +2168,7 @@
     </row>
     <row r="9" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s">
         <v>122</v>
@@ -2146,14 +2182,14 @@
       <c r="H9" t="s">
         <v>124</v>
       </c>
-      <c r="I9" s="6">
-        <v>12</v>
+      <c r="I9">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J9">
         <v>1000</v>
       </c>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4">
         <v>0.37895014829661294</v>
@@ -2314,7 +2350,7 @@
     </row>
     <row r="10" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B10" t="s">
         <v>122</v>
@@ -2328,8 +2364,8 @@
       <c r="H10" t="s">
         <v>124</v>
       </c>
-      <c r="I10" s="6">
-        <v>12</v>
+      <c r="I10">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J10">
         <v>1000</v>
@@ -2394,7 +2430,7 @@
     </row>
     <row r="11" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B11" t="s">
         <v>122</v>
@@ -2408,8 +2444,8 @@
       <c r="H11" t="s">
         <v>124</v>
       </c>
-      <c r="I11" s="6">
-        <v>12</v>
+      <c r="I11">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J11">
         <v>1000</v>
@@ -2577,7 +2613,7 @@
     </row>
     <row r="12" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B12" t="s">
         <v>122</v>
@@ -2600,14 +2636,14 @@
       <c r="H12" t="s">
         <v>124</v>
       </c>
-      <c r="I12" s="6">
-        <v>12</v>
+      <c r="I12">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J12">
         <v>1000</v>
       </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="R12">
@@ -2659,7 +2695,7 @@
     </row>
     <row r="13" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s">
         <v>122</v>
@@ -2673,8 +2709,8 @@
       <c r="H13" t="s">
         <v>124</v>
       </c>
-      <c r="I13" s="6">
-        <v>12</v>
+      <c r="I13">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J13">
         <v>1000</v>
@@ -2739,7 +2775,7 @@
     </row>
     <row r="14" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B14" t="s">
         <v>122</v>
@@ -2753,8 +2789,8 @@
       <c r="H14" t="s">
         <v>124</v>
       </c>
-      <c r="I14" s="6">
-        <v>12</v>
+      <c r="I14">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J14">
         <v>1000</v>
@@ -2870,7 +2906,7 @@
     </row>
     <row r="15" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B15" t="s">
         <v>122</v>
@@ -2884,14 +2920,14 @@
       <c r="H15" t="s">
         <v>124</v>
       </c>
-      <c r="I15" s="6">
-        <v>12</v>
+      <c r="I15">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J15">
         <v>1000</v>
       </c>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="R15">
@@ -2992,7 +3028,7 @@
     </row>
     <row r="16" spans="1:150" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B16" t="s">
         <v>122</v>
@@ -3006,12 +3042,14 @@
       <c r="H16" t="s">
         <v>124</v>
       </c>
-      <c r="I16" s="6">
-        <v>12</v>
+      <c r="I16">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J16">
         <v>1000</v>
       </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
       <c r="P16" s="4">
         <v>0.75843704767032827</v>
       </c>
@@ -3110,7 +3148,7 @@
     </row>
     <row r="17" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B17" t="s">
         <v>122</v>
@@ -3124,8 +3162,8 @@
       <c r="H17" t="s">
         <v>124</v>
       </c>
-      <c r="I17" s="6">
-        <v>12</v>
+      <c r="I17">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J17">
         <v>1000</v>
@@ -3190,7 +3228,7 @@
     </row>
     <row r="18" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B18" t="s">
         <v>122</v>
@@ -3204,14 +3242,14 @@
       <c r="H18" t="s">
         <v>124</v>
       </c>
-      <c r="I18" s="6">
-        <v>12</v>
+      <c r="I18">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J18">
         <v>1000</v>
       </c>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="R18">
@@ -3312,7 +3350,7 @@
     </row>
     <row r="19" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B19" t="s">
         <v>122</v>
@@ -3326,12 +3364,14 @@
       <c r="H19" t="s">
         <v>124</v>
       </c>
-      <c r="I19" s="6">
-        <v>12</v>
+      <c r="I19">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J19">
         <v>1000</v>
       </c>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
       <c r="P19" s="4">
         <v>0.82875302679901452</v>
       </c>
@@ -3430,7 +3470,7 @@
     </row>
     <row r="20" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B20" t="s">
         <v>122</v>
@@ -3444,8 +3484,8 @@
       <c r="H20" t="s">
         <v>124</v>
       </c>
-      <c r="I20" s="6">
-        <v>12</v>
+      <c r="I20">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J20">
         <v>1000</v>
@@ -3510,7 +3550,7 @@
     </row>
     <row r="21" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s">
         <v>122</v>
@@ -3524,12 +3564,14 @@
       <c r="H21" t="s">
         <v>124</v>
       </c>
-      <c r="I21" s="6">
-        <v>12</v>
+      <c r="I21">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J21">
         <v>1000</v>
       </c>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
       <c r="P21" s="4">
         <v>0.84226048678169019</v>
       </c>
@@ -3570,7 +3612,7 @@
     </row>
     <row r="22" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B22" t="s">
         <v>122</v>
@@ -3584,8 +3626,8 @@
       <c r="H22" t="s">
         <v>124</v>
       </c>
-      <c r="I22" s="6">
-        <v>12</v>
+      <c r="I22">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J22">
         <v>1000</v>
@@ -3699,7 +3741,7 @@
     </row>
     <row r="23" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B23" t="s">
         <v>122</v>
@@ -3713,8 +3755,8 @@
       <c r="H23" t="s">
         <v>124</v>
       </c>
-      <c r="I23" s="6">
-        <v>12</v>
+      <c r="I23">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J23">
         <v>1000</v>
@@ -3833,7 +3875,7 @@
     </row>
     <row r="24" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B24" t="s">
         <v>122</v>
@@ -3847,8 +3889,8 @@
       <c r="H24" t="s">
         <v>124</v>
       </c>
-      <c r="I24" s="6">
-        <v>12</v>
+      <c r="I24">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J24">
         <v>1000</v>
@@ -3913,7 +3955,7 @@
     </row>
     <row r="25" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B25" t="s">
         <v>122</v>
@@ -3927,14 +3969,14 @@
       <c r="H25" t="s">
         <v>124</v>
       </c>
-      <c r="I25" s="6">
-        <v>12</v>
+      <c r="I25">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J25">
         <v>1000</v>
       </c>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="R25">
@@ -4035,7 +4077,7 @@
     </row>
     <row r="26" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B26" t="s">
         <v>122</v>
@@ -4049,12 +4091,14 @@
       <c r="H26" t="s">
         <v>124</v>
       </c>
-      <c r="I26" s="6">
-        <v>12</v>
+      <c r="I26">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J26">
         <v>1000</v>
       </c>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
       <c r="P26" s="4">
         <v>0.89868729098399325</v>
       </c>
@@ -4153,7 +4197,7 @@
     </row>
     <row r="27" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B27" t="s">
         <v>122</v>
@@ -4167,8 +4211,8 @@
       <c r="H27" t="s">
         <v>124</v>
       </c>
-      <c r="I27" s="6">
-        <v>12</v>
+      <c r="I27">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J27">
         <v>1000</v>
@@ -4234,7 +4278,7 @@
     </row>
     <row r="28" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B28" t="s">
         <v>122</v>
@@ -4248,14 +4292,14 @@
       <c r="H28" t="s">
         <v>124</v>
       </c>
-      <c r="I28" s="6">
-        <v>12</v>
+      <c r="I28">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J28">
         <v>1000</v>
       </c>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="R28">
@@ -4412,7 +4456,7 @@
     </row>
     <row r="29" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B29" t="s">
         <v>122</v>
@@ -4426,12 +4470,14 @@
       <c r="H29" t="s">
         <v>124</v>
       </c>
-      <c r="I29" s="6">
-        <v>12</v>
+      <c r="I29">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J29">
         <v>1000</v>
       </c>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
       <c r="P29" s="4">
         <v>0.80815371934306313</v>
       </c>
@@ -4472,7 +4518,7 @@
     </row>
     <row r="30" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B30" t="s">
         <v>122</v>
@@ -4489,12 +4535,14 @@
       <c r="H30" t="s">
         <v>124</v>
       </c>
-      <c r="I30" s="6">
-        <v>12</v>
+      <c r="I30">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J30">
         <v>1000</v>
       </c>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
       <c r="P30" s="4"/>
       <c r="R30">
         <v>53</v>
@@ -4536,7 +4584,7 @@
     </row>
     <row r="31" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B31" t="s">
         <v>122</v>
@@ -4550,12 +4598,14 @@
       <c r="H31" t="s">
         <v>124</v>
       </c>
-      <c r="I31" s="6">
-        <v>12</v>
+      <c r="I31">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J31">
         <v>1000</v>
       </c>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
       <c r="P31" s="4"/>
       <c r="R31">
         <v>53</v>
@@ -4653,7 +4703,7 @@
     </row>
     <row r="32" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B32" t="s">
         <v>122</v>
@@ -4670,14 +4720,14 @@
       <c r="H32" t="s">
         <v>124</v>
       </c>
-      <c r="I32" s="6">
-        <v>12</v>
+      <c r="I32">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J32">
         <v>1000</v>
       </c>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
       <c r="O32" s="4"/>
       <c r="P32" s="4">
         <v>0.83046900346417196</v>
@@ -4781,7 +4831,7 @@
     </row>
     <row r="33" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B33" t="s">
         <v>122</v>
@@ -4795,14 +4845,14 @@
       <c r="H33" t="s">
         <v>124</v>
       </c>
-      <c r="I33" s="6">
-        <v>12</v>
+      <c r="I33">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J33">
         <v>1000</v>
       </c>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="R33">
@@ -4915,7 +4965,7 @@
     </row>
     <row r="34" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B34" t="s">
         <v>122</v>
@@ -4932,12 +4982,14 @@
       <c r="H34" t="s">
         <v>124</v>
       </c>
-      <c r="I34" s="6">
-        <v>12</v>
+      <c r="I34">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J34">
         <v>1000</v>
       </c>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
       <c r="P34" s="4"/>
       <c r="R34">
         <v>53</v>
@@ -5037,7 +5089,7 @@
     </row>
     <row r="35" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B35" t="s">
         <v>122</v>
@@ -5060,14 +5112,14 @@
       <c r="H35" t="s">
         <v>124</v>
       </c>
-      <c r="I35" s="6">
-        <v>12</v>
+      <c r="I35">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J35">
         <v>1000</v>
       </c>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="R35">
@@ -5120,7 +5172,7 @@
     </row>
     <row r="36" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B36" t="s">
         <v>122</v>
@@ -5134,12 +5186,14 @@
       <c r="H36" t="s">
         <v>124</v>
       </c>
-      <c r="I36" s="6">
-        <v>12</v>
+      <c r="I36">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J36">
         <v>1000</v>
       </c>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
       <c r="P36" s="4">
         <v>0.91878648348018765</v>
       </c>
@@ -5238,7 +5292,7 @@
     </row>
     <row r="37" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B37" t="s">
         <v>122</v>
@@ -5255,12 +5309,14 @@
       <c r="H37" t="s">
         <v>124</v>
       </c>
-      <c r="I37" s="6">
-        <v>12</v>
+      <c r="I37">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J37">
         <v>1000</v>
       </c>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
       <c r="P37" s="4"/>
       <c r="R37">
         <v>53</v>
@@ -5302,7 +5358,7 @@
     </row>
     <row r="38" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B38" t="s">
         <v>122</v>
@@ -5316,12 +5372,14 @@
       <c r="H38" t="s">
         <v>124</v>
       </c>
-      <c r="I38" s="6">
-        <v>12</v>
+      <c r="I38">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J38">
         <v>1000</v>
       </c>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
       <c r="P38" s="4"/>
       <c r="R38">
         <v>53</v>
@@ -5412,7 +5470,7 @@
     </row>
     <row r="39" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B39" t="s">
         <v>122</v>
@@ -5426,12 +5484,14 @@
       <c r="H39" t="s">
         <v>124</v>
       </c>
-      <c r="I39" s="6">
-        <v>12</v>
+      <c r="I39">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J39">
         <v>1000</v>
       </c>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
       <c r="P39" s="4"/>
       <c r="R39">
         <v>53</v>
@@ -5538,7 +5598,7 @@
     </row>
     <row r="40" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B40" t="s">
         <v>122</v>
@@ -5555,12 +5615,14 @@
       <c r="H40" t="s">
         <v>124</v>
       </c>
-      <c r="I40" s="6">
-        <v>12</v>
+      <c r="I40">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J40">
         <v>1000</v>
       </c>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
       <c r="P40" s="4">
         <v>0.85958384604401195</v>
       </c>
@@ -5604,7 +5666,7 @@
     </row>
     <row r="41" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B41" t="s">
         <v>122</v>
@@ -5621,12 +5683,14 @@
       <c r="H41" t="s">
         <v>124</v>
       </c>
-      <c r="I41" s="6">
-        <v>12</v>
+      <c r="I41">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J41">
         <v>1000</v>
       </c>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
       <c r="R41">
         <v>53</v>
       </c>
@@ -5667,7 +5731,7 @@
     </row>
     <row r="42" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B42" t="s">
         <v>122</v>
@@ -5681,12 +5745,14 @@
       <c r="H42" t="s">
         <v>124</v>
       </c>
-      <c r="I42" s="6">
-        <v>12</v>
+      <c r="I42">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J42">
         <v>1000</v>
       </c>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
       <c r="R42">
         <v>53</v>
       </c>
@@ -5776,7 +5842,7 @@
     </row>
     <row r="43" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B43" t="s">
         <v>122</v>
@@ -5793,12 +5859,14 @@
       <c r="H43" t="s">
         <v>124</v>
       </c>
-      <c r="I43" s="6">
-        <v>12</v>
+      <c r="I43">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J43">
         <v>1000</v>
       </c>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
       <c r="R43">
         <v>53</v>
       </c>
@@ -5832,7 +5900,7 @@
     </row>
     <row r="44" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B44" t="s">
         <v>122</v>
@@ -5855,12 +5923,14 @@
       <c r="H44" t="s">
         <v>124</v>
       </c>
-      <c r="I44" s="6">
-        <v>12</v>
+      <c r="I44">
+        <v>8.6999999999999993</v>
       </c>
       <c r="J44">
         <v>1000</v>
       </c>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
       <c r="R44">
         <v>53</v>
       </c>
@@ -5908,6 +5978,1560 @@
         <v>100</v>
       </c>
     </row>
+    <row r="45" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" s="7">
+        <v>37539</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>72</v>
+      </c>
+      <c r="G45" s="15">
+        <v>0</v>
+      </c>
+      <c r="H45" t="s">
+        <v>124</v>
+      </c>
+      <c r="I45" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J45" s="14">
+        <v>380</v>
+      </c>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="AU45"/>
+      <c r="AV45"/>
+      <c r="AW45"/>
+      <c r="AY45"/>
+      <c r="AZ45"/>
+      <c r="BA45"/>
+      <c r="BB45"/>
+      <c r="BC45"/>
+      <c r="BD45"/>
+    </row>
+    <row r="46" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>163</v>
+      </c>
+      <c r="B46" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46" s="7">
+        <v>37594</v>
+      </c>
+      <c r="G46" s="12">
+        <v>55</v>
+      </c>
+      <c r="H46" t="s">
+        <v>124</v>
+      </c>
+      <c r="I46" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J46" s="14">
+        <v>380</v>
+      </c>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="AC46">
+        <v>28.166666666666668</v>
+      </c>
+      <c r="AJ46">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="AK46">
+        <v>0.44165199999999999</v>
+      </c>
+      <c r="AQ46">
+        <v>1.1266632653061224E-2</v>
+      </c>
+      <c r="AR46">
+        <v>4.0389981787596098E-2</v>
+      </c>
+      <c r="AS46">
+        <v>1.5832872860737672</v>
+      </c>
+      <c r="BH46">
+        <v>0.3666666666666667</v>
+      </c>
+      <c r="BK46">
+        <v>67.733333333333334</v>
+      </c>
+      <c r="BM46">
+        <v>5.4133858267716543E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>163</v>
+      </c>
+      <c r="B47" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" s="7">
+        <v>37599</v>
+      </c>
+      <c r="G47">
+        <v>60</v>
+      </c>
+      <c r="H47" t="s">
+        <v>124</v>
+      </c>
+      <c r="I47" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J47" s="14">
+        <v>380</v>
+      </c>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="CM47">
+        <v>441.18316907705798</v>
+      </c>
+      <c r="CO47">
+        <v>22.334272169487985</v>
+      </c>
+      <c r="CQ47">
+        <v>27.920979108836587</v>
+      </c>
+      <c r="CS47">
+        <v>28.544532627935649</v>
+      </c>
+      <c r="CU47">
+        <v>32.794861336223256</v>
+      </c>
+      <c r="CW47">
+        <v>44.944300368066116</v>
+      </c>
+      <c r="CY47">
+        <v>67.461290326927326</v>
+      </c>
+      <c r="DA47">
+        <v>74.449906101622418</v>
+      </c>
+      <c r="DC47">
+        <v>71.126829510578901</v>
+      </c>
+      <c r="DE47">
+        <v>71.606197527379805</v>
+      </c>
+    </row>
+    <row r="48" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>163</v>
+      </c>
+      <c r="B48" t="s">
+        <v>164</v>
+      </c>
+      <c r="C48" s="7">
+        <v>37606</v>
+      </c>
+      <c r="G48" s="12">
+        <v>67</v>
+      </c>
+      <c r="H48" t="s">
+        <v>124</v>
+      </c>
+      <c r="I48" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J48" s="14">
+        <v>380</v>
+      </c>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="AC48">
+        <v>69.058915088606554</v>
+      </c>
+      <c r="AJ48">
+        <v>83.005011704517287</v>
+      </c>
+      <c r="AK48">
+        <v>0.74578656335662108</v>
+      </c>
+      <c r="AQ48">
+        <v>8.9848377590920087E-3</v>
+      </c>
+      <c r="AR48">
+        <v>2.8234555681406835E-2</v>
+      </c>
+      <c r="AS48">
+        <v>2.3436096248070193</v>
+      </c>
+      <c r="BH48">
+        <v>13.82774659500558</v>
+      </c>
+      <c r="BK48">
+        <v>165.89167338812942</v>
+      </c>
+      <c r="BM48">
+        <v>8.3354072646270871E-2</v>
+      </c>
+      <c r="CM48">
+        <v>482.47525544134066</v>
+      </c>
+      <c r="CO48">
+        <v>27.542072141674293</v>
+      </c>
+      <c r="CQ48">
+        <v>38.023417429303819</v>
+      </c>
+      <c r="CS48">
+        <v>40.177331916998078</v>
+      </c>
+      <c r="CU48">
+        <v>39.651245830763195</v>
+      </c>
+      <c r="CW48">
+        <v>49.387595015320187</v>
+      </c>
+      <c r="CY48">
+        <v>67.77054363437621</v>
+      </c>
+      <c r="DA48">
+        <v>75.264425486101914</v>
+      </c>
+      <c r="DC48">
+        <v>72.652276038619036</v>
+      </c>
+      <c r="DE48">
+        <v>72.006347948183944</v>
+      </c>
+    </row>
+    <row r="49" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>163</v>
+      </c>
+      <c r="B49" t="s">
+        <v>164</v>
+      </c>
+      <c r="C49" s="7">
+        <v>37608</v>
+      </c>
+      <c r="G49">
+        <v>69</v>
+      </c>
+      <c r="H49" t="s">
+        <v>124</v>
+      </c>
+      <c r="I49" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J49" s="14">
+        <v>380</v>
+      </c>
+      <c r="M49" s="1">
+        <v>285</v>
+      </c>
+      <c r="N49" s="1">
+        <v>14.166666666666666</v>
+      </c>
+    </row>
+    <row r="50" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>163</v>
+      </c>
+      <c r="B50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C50" s="7">
+        <v>37613</v>
+      </c>
+      <c r="G50" s="12">
+        <v>74</v>
+      </c>
+      <c r="H50" t="s">
+        <v>124</v>
+      </c>
+      <c r="I50" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J50" s="14">
+        <v>380</v>
+      </c>
+      <c r="M50" s="1">
+        <v>356.66666666666663</v>
+      </c>
+      <c r="N50" s="1">
+        <v>16.069444444444446</v>
+      </c>
+      <c r="AC50">
+        <v>107.40503651758718</v>
+      </c>
+      <c r="AJ50">
+        <v>100.24208306991689</v>
+      </c>
+      <c r="AK50">
+        <v>1.2582825232981376</v>
+      </c>
+      <c r="AQ50">
+        <v>1.2552437905949242E-2</v>
+      </c>
+      <c r="AR50">
+        <v>2.9918069651741298E-2</v>
+      </c>
+      <c r="AS50">
+        <v>2.9990496233214108</v>
+      </c>
+      <c r="BH50">
+        <v>20.036315645275355</v>
+      </c>
+      <c r="BK50">
+        <v>227.6834352327794</v>
+      </c>
+      <c r="BM50">
+        <v>8.8000761341248165E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>163</v>
+      </c>
+      <c r="B51" t="s">
+        <v>164</v>
+      </c>
+      <c r="C51" s="7">
+        <v>37613</v>
+      </c>
+      <c r="G51">
+        <v>74</v>
+      </c>
+      <c r="H51" t="s">
+        <v>124</v>
+      </c>
+      <c r="I51" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J51" s="14">
+        <v>380</v>
+      </c>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="CM51">
+        <v>461.38669219534501</v>
+      </c>
+      <c r="CO51">
+        <v>25.555957372233831</v>
+      </c>
+      <c r="CQ51">
+        <v>33.178612816857473</v>
+      </c>
+      <c r="CS51">
+        <v>34.733661217733662</v>
+      </c>
+      <c r="CU51">
+        <v>36.151453064034627</v>
+      </c>
+      <c r="CW51">
+        <v>46.555312055884819</v>
+      </c>
+      <c r="CY51">
+        <v>65.479580914252011</v>
+      </c>
+      <c r="DA51">
+        <v>76.310503997341144</v>
+      </c>
+      <c r="DC51">
+        <v>71.742289294861408</v>
+      </c>
+      <c r="DE51">
+        <v>71.679321462146035</v>
+      </c>
+    </row>
+    <row r="52" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>163</v>
+      </c>
+      <c r="B52" t="s">
+        <v>164</v>
+      </c>
+      <c r="C52" s="7">
+        <v>37620</v>
+      </c>
+      <c r="G52">
+        <v>81</v>
+      </c>
+      <c r="H52" t="s">
+        <v>124</v>
+      </c>
+      <c r="I52" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J52" s="14">
+        <v>380</v>
+      </c>
+      <c r="M52" s="1">
+        <v>456.25</v>
+      </c>
+      <c r="N52" s="1">
+        <v>18.041666666666668</v>
+      </c>
+    </row>
+    <row r="53" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>163</v>
+      </c>
+      <c r="B53" t="s">
+        <v>164</v>
+      </c>
+      <c r="C53" s="7">
+        <v>37621</v>
+      </c>
+      <c r="G53">
+        <v>82</v>
+      </c>
+      <c r="H53" t="s">
+        <v>124</v>
+      </c>
+      <c r="I53" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J53" s="14">
+        <v>380</v>
+      </c>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="CM53">
+        <v>408.87650658986809</v>
+      </c>
+      <c r="CO53">
+        <v>23.006534955025746</v>
+      </c>
+      <c r="CQ53">
+        <v>28.28750421328056</v>
+      </c>
+      <c r="CS53">
+        <v>30.578118238717931</v>
+      </c>
+      <c r="CU53">
+        <v>31.539223970133133</v>
+      </c>
+      <c r="CW53">
+        <v>40.015934340142039</v>
+      </c>
+      <c r="CY53">
+        <v>57.18367079470331</v>
+      </c>
+      <c r="DA53">
+        <v>66.481299017251601</v>
+      </c>
+      <c r="DC53">
+        <v>65.845461116481573</v>
+      </c>
+      <c r="DE53">
+        <v>65.938759944132258</v>
+      </c>
+    </row>
+    <row r="54" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>163</v>
+      </c>
+      <c r="B54" t="s">
+        <v>164</v>
+      </c>
+      <c r="C54" s="7">
+        <v>37623</v>
+      </c>
+      <c r="G54" s="12">
+        <v>84</v>
+      </c>
+      <c r="H54" t="s">
+        <v>124</v>
+      </c>
+      <c r="I54" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J54" s="14">
+        <v>380</v>
+      </c>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="AC54">
+        <v>163.05283592784707</v>
+      </c>
+      <c r="AJ54">
+        <v>154.2014351487644</v>
+      </c>
+      <c r="AK54">
+        <v>2.0754754761103751</v>
+      </c>
+      <c r="AQ54">
+        <v>1.345950816935056E-2</v>
+      </c>
+      <c r="AR54">
+        <v>3.1896323007026821E-2</v>
+      </c>
+      <c r="AS54">
+        <v>4.9184587836520883</v>
+      </c>
+      <c r="BH54">
+        <v>51.020777672873862</v>
+      </c>
+      <c r="BK54">
+        <v>368.27504874948534</v>
+      </c>
+      <c r="BM54">
+        <v>0.13853987080069638</v>
+      </c>
+    </row>
+    <row r="55" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>163</v>
+      </c>
+      <c r="B55" t="s">
+        <v>164</v>
+      </c>
+      <c r="C55" s="7">
+        <v>37627</v>
+      </c>
+      <c r="G55">
+        <v>88</v>
+      </c>
+      <c r="H55" t="s">
+        <v>124</v>
+      </c>
+      <c r="I55" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J55" s="14">
+        <v>380</v>
+      </c>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="CM55">
+        <v>475.48820047784938</v>
+      </c>
+      <c r="CO55">
+        <v>25.719230320622518</v>
+      </c>
+      <c r="CQ55">
+        <v>34.918861782779999</v>
+      </c>
+      <c r="CS55">
+        <v>39.021567503609475</v>
+      </c>
+      <c r="CU55">
+        <v>39.832024447268623</v>
+      </c>
+      <c r="CW55">
+        <v>49.032131443539868</v>
+      </c>
+      <c r="CY55">
+        <v>66.832119804876172</v>
+      </c>
+      <c r="DA55">
+        <v>75.28880013102399</v>
+      </c>
+      <c r="DC55">
+        <v>72.835085875534631</v>
+      </c>
+      <c r="DE55">
+        <v>72.008379168594118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>163</v>
+      </c>
+      <c r="B56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" s="7">
+        <v>37628</v>
+      </c>
+      <c r="G56">
+        <v>89</v>
+      </c>
+      <c r="H56" t="s">
+        <v>124</v>
+      </c>
+      <c r="I56" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J56" s="14">
+        <v>380</v>
+      </c>
+      <c r="M56" s="1">
+        <v>512.5</v>
+      </c>
+      <c r="N56" s="1">
+        <v>19.652777777777775</v>
+      </c>
+    </row>
+    <row r="57" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>163</v>
+      </c>
+      <c r="B57" t="s">
+        <v>164</v>
+      </c>
+      <c r="C57" s="7">
+        <v>37631</v>
+      </c>
+      <c r="G57" s="12">
+        <v>92</v>
+      </c>
+      <c r="H57" t="s">
+        <v>124</v>
+      </c>
+      <c r="I57" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J57" s="14">
+        <v>380</v>
+      </c>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="AC57">
+        <v>234.79999999999998</v>
+      </c>
+      <c r="AJ57">
+        <v>187.80000000000004</v>
+      </c>
+      <c r="AK57">
+        <v>2.7587953333333335</v>
+      </c>
+      <c r="AQ57">
+        <v>1.4690070997515084E-2</v>
+      </c>
+      <c r="AR57">
+        <v>2.9367473950285786E-2</v>
+      </c>
+      <c r="AS57">
+        <v>5.5152116078636721</v>
+      </c>
+      <c r="BH57">
+        <v>108.8</v>
+      </c>
+      <c r="BK57">
+        <v>531.4</v>
+      </c>
+      <c r="BM57">
+        <v>0.20474219044034625</v>
+      </c>
+    </row>
+    <row r="58" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>163</v>
+      </c>
+      <c r="B58" t="s">
+        <v>164</v>
+      </c>
+      <c r="C58" s="7">
+        <v>37634</v>
+      </c>
+      <c r="G58">
+        <v>95</v>
+      </c>
+      <c r="H58" t="s">
+        <v>124</v>
+      </c>
+      <c r="I58" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J58" s="14">
+        <v>380</v>
+      </c>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="CM58">
+        <v>436.11211502542864</v>
+      </c>
+      <c r="CO58">
+        <v>23.226042813231285</v>
+      </c>
+      <c r="CQ58">
+        <v>29.185236632860441</v>
+      </c>
+      <c r="CS58">
+        <v>29.839435639421122</v>
+      </c>
+      <c r="CU58">
+        <v>33.329072304098837</v>
+      </c>
+      <c r="CW58">
+        <v>42.237699171510215</v>
+      </c>
+      <c r="CY58">
+        <v>61.29044272082087</v>
+      </c>
+      <c r="DA58">
+        <v>71.575729221227206</v>
+      </c>
+      <c r="DC58">
+        <v>72.394311046527037</v>
+      </c>
+      <c r="DE58">
+        <v>73.034145475731634</v>
+      </c>
+    </row>
+    <row r="59" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>163</v>
+      </c>
+      <c r="B59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C59" s="7">
+        <v>37636</v>
+      </c>
+      <c r="G59">
+        <v>97</v>
+      </c>
+      <c r="H59" t="s">
+        <v>124</v>
+      </c>
+      <c r="I59" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J59" s="14">
+        <v>380</v>
+      </c>
+      <c r="M59" s="1">
+        <v>550</v>
+      </c>
+      <c r="N59" s="1">
+        <v>21.027777777777775</v>
+      </c>
+    </row>
+    <row r="60" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>163</v>
+      </c>
+      <c r="B60" t="s">
+        <v>164</v>
+      </c>
+      <c r="C60" s="7">
+        <v>37642</v>
+      </c>
+      <c r="G60" s="13">
+        <v>103</v>
+      </c>
+      <c r="H60" t="s">
+        <v>124</v>
+      </c>
+      <c r="I60" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J60" s="14">
+        <v>380</v>
+      </c>
+      <c r="M60" s="1">
+        <v>554.58333333333337</v>
+      </c>
+      <c r="N60" s="1">
+        <v>21.375</v>
+      </c>
+      <c r="AC60">
+        <v>255.3324384499268</v>
+      </c>
+      <c r="AJ60">
+        <v>172.24948076140012</v>
+      </c>
+      <c r="AK60">
+        <v>2.4590574584663005</v>
+      </c>
+      <c r="AQ60">
+        <v>1.4276138584548684E-2</v>
+      </c>
+      <c r="AR60">
+        <v>2.9680706028275522E-2</v>
+      </c>
+      <c r="AS60">
+        <v>5.1124862020022173</v>
+      </c>
+      <c r="BH60">
+        <v>309.92831170209831</v>
+      </c>
+      <c r="BK60">
+        <v>737.51023091342518</v>
+      </c>
+      <c r="BM60">
+        <v>0.42023594888744015</v>
+      </c>
+    </row>
+    <row r="61" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>163</v>
+      </c>
+      <c r="B61" t="s">
+        <v>164</v>
+      </c>
+      <c r="C61" s="7">
+        <v>37645</v>
+      </c>
+      <c r="G61">
+        <v>106</v>
+      </c>
+      <c r="H61" t="s">
+        <v>124</v>
+      </c>
+      <c r="I61" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J61" s="14">
+        <v>380</v>
+      </c>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="CM61">
+        <v>443.730802273839</v>
+      </c>
+      <c r="CO61">
+        <v>23.958374706982497</v>
+      </c>
+      <c r="CQ61">
+        <v>30.718818401610406</v>
+      </c>
+      <c r="CS61">
+        <v>32.833454524016553</v>
+      </c>
+      <c r="CU61">
+        <v>35.591851841031882</v>
+      </c>
+      <c r="CW61">
+        <v>44.534247747762386</v>
+      </c>
+      <c r="CY61">
+        <v>61.494834274594574</v>
+      </c>
+      <c r="DA61">
+        <v>71.25479639641982</v>
+      </c>
+      <c r="DC61">
+        <v>71.923067911366829</v>
+      </c>
+      <c r="DE61">
+        <v>71.421356470054036</v>
+      </c>
+    </row>
+    <row r="62" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>163</v>
+      </c>
+      <c r="B62" t="s">
+        <v>164</v>
+      </c>
+      <c r="C62" s="7">
+        <v>37650</v>
+      </c>
+      <c r="G62">
+        <v>111</v>
+      </c>
+      <c r="H62" t="s">
+        <v>124</v>
+      </c>
+      <c r="I62" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J62" s="14">
+        <v>380</v>
+      </c>
+      <c r="M62" s="1">
+        <v>561.25</v>
+      </c>
+      <c r="N62" s="1">
+        <v>21.625</v>
+      </c>
+    </row>
+    <row r="63" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>163</v>
+      </c>
+      <c r="B63" t="s">
+        <v>164</v>
+      </c>
+      <c r="C63" s="7">
+        <v>37652</v>
+      </c>
+      <c r="G63" s="13">
+        <v>113</v>
+      </c>
+      <c r="H63" t="s">
+        <v>124</v>
+      </c>
+      <c r="I63" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J63" s="14">
+        <v>380</v>
+      </c>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="AC63">
+        <v>268.98330719342749</v>
+      </c>
+      <c r="AJ63">
+        <v>173.42593278609607</v>
+      </c>
+      <c r="AK63">
+        <v>2.6444006755744387</v>
+      </c>
+      <c r="AQ63">
+        <v>1.5248011834747046E-2</v>
+      </c>
+      <c r="AR63">
+        <v>2.2503378117184086E-2</v>
+      </c>
+      <c r="AS63">
+        <v>3.9026693408108724</v>
+      </c>
+      <c r="BH63">
+        <v>456.71547635604867</v>
+      </c>
+      <c r="BK63">
+        <v>899.1247163355722</v>
+      </c>
+      <c r="BM63">
+        <v>0.50795564626163925</v>
+      </c>
+    </row>
+    <row r="64" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>163</v>
+      </c>
+      <c r="B64" t="s">
+        <v>164</v>
+      </c>
+      <c r="C64" s="7">
+        <v>37655</v>
+      </c>
+      <c r="G64">
+        <v>116</v>
+      </c>
+      <c r="H64" t="s">
+        <v>124</v>
+      </c>
+      <c r="I64" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J64" s="14">
+        <v>380</v>
+      </c>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="CM64">
+        <v>461.56463903673188</v>
+      </c>
+      <c r="CO64">
+        <v>24.451069200946005</v>
+      </c>
+      <c r="CQ64">
+        <v>33.256934126299399</v>
+      </c>
+      <c r="CS64">
+        <v>37.058392977176993</v>
+      </c>
+      <c r="CU64">
+        <v>38.230407153846983</v>
+      </c>
+      <c r="CW64">
+        <v>47.890839475573756</v>
+      </c>
+      <c r="CY64">
+        <v>65.088570985293643</v>
+      </c>
+      <c r="DA64">
+        <v>72.516184271137433</v>
+      </c>
+      <c r="DC64">
+        <v>71.502605286460962</v>
+      </c>
+      <c r="DE64">
+        <v>71.569635559996684</v>
+      </c>
+    </row>
+    <row r="65" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>163</v>
+      </c>
+      <c r="B65" t="s">
+        <v>164</v>
+      </c>
+      <c r="C65" s="7">
+        <v>37657</v>
+      </c>
+      <c r="G65">
+        <v>118</v>
+      </c>
+      <c r="H65" t="s">
+        <v>124</v>
+      </c>
+      <c r="I65" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J65" s="14">
+        <v>380</v>
+      </c>
+      <c r="M65" s="1">
+        <v>561.25</v>
+      </c>
+      <c r="N65" s="1">
+        <v>21.833333333333332</v>
+      </c>
+    </row>
+    <row r="66" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>163</v>
+      </c>
+      <c r="B66" t="s">
+        <v>164</v>
+      </c>
+      <c r="C66" s="7">
+        <v>37662</v>
+      </c>
+      <c r="G66" s="13">
+        <v>123</v>
+      </c>
+      <c r="H66" t="s">
+        <v>124</v>
+      </c>
+      <c r="I66" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J66" s="14">
+        <v>380</v>
+      </c>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="AC66">
+        <v>253.15990812250848</v>
+      </c>
+      <c r="AJ66">
+        <v>177.13490031457911</v>
+      </c>
+      <c r="AK66">
+        <v>2.6083667777078143</v>
+      </c>
+      <c r="AQ66">
+        <v>1.4725312589870988E-2</v>
+      </c>
+      <c r="AR66">
+        <v>1.8026579901579902E-2</v>
+      </c>
+      <c r="AS66">
+        <v>3.1931364338791512</v>
+      </c>
+      <c r="BH66">
+        <v>628.03692962352477</v>
+      </c>
+      <c r="BK66">
+        <v>1058.3317380606122</v>
+      </c>
+      <c r="BM66">
+        <v>0.59342161539480942</v>
+      </c>
+      <c r="CM66">
+        <v>421.00743659410091</v>
+      </c>
+      <c r="CO66">
+        <v>23.317744058216707</v>
+      </c>
+      <c r="CQ66">
+        <v>29.504080157104671</v>
+      </c>
+      <c r="CS66">
+        <v>30.357396844015312</v>
+      </c>
+      <c r="CU66">
+        <v>32.72173740145702</v>
+      </c>
+      <c r="CW66">
+        <v>41.507729336604193</v>
+      </c>
+      <c r="CY66">
+        <v>57.636277202919132</v>
+      </c>
+      <c r="DA66">
+        <v>66.690644134760433</v>
+      </c>
+      <c r="DC66">
+        <v>68.370463413973752</v>
+      </c>
+      <c r="DE66">
+        <v>70.901364045049675</v>
+      </c>
+    </row>
+    <row r="67" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>163</v>
+      </c>
+      <c r="B67" t="s">
+        <v>164</v>
+      </c>
+      <c r="C67" s="7">
+        <v>37670</v>
+      </c>
+      <c r="G67">
+        <v>131</v>
+      </c>
+      <c r="H67" t="s">
+        <v>124</v>
+      </c>
+      <c r="I67" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J67" s="14">
+        <v>380</v>
+      </c>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="CM67">
+        <v>464.52009603585321</v>
+      </c>
+      <c r="CO67">
+        <v>25.277338955413999</v>
+      </c>
+      <c r="CQ67">
+        <v>34.64701104420093</v>
+      </c>
+      <c r="CS67">
+        <v>38.235485204872425</v>
+      </c>
+      <c r="CU67">
+        <v>39.662417543019153</v>
+      </c>
+      <c r="CW67">
+        <v>47.909882166919125</v>
+      </c>
+      <c r="CY67">
+        <v>65.131226613907302</v>
+      </c>
+      <c r="DA67">
+        <v>72.181032903458842</v>
+      </c>
+      <c r="DC67">
+        <v>70.206686664770416</v>
+      </c>
+      <c r="DE67">
+        <v>71.26901493929104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" t="s">
+        <v>164</v>
+      </c>
+      <c r="C68" s="7">
+        <v>37677</v>
+      </c>
+      <c r="G68" s="13">
+        <v>138</v>
+      </c>
+      <c r="H68" t="s">
+        <v>124</v>
+      </c>
+      <c r="I68" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J68" s="14">
+        <v>380</v>
+      </c>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="AC68">
+        <v>272.7232065679861</v>
+      </c>
+      <c r="AJ68">
+        <v>190.83354129335666</v>
+      </c>
+      <c r="AK68">
+        <v>2.4936474491697287</v>
+      </c>
+      <c r="AQ68">
+        <v>1.3067133965388181E-2</v>
+      </c>
+      <c r="AR68">
+        <v>1.4813365831153892E-2</v>
+      </c>
+      <c r="AS68">
+        <v>2.8268870600331049</v>
+      </c>
+      <c r="BH68">
+        <v>708.21831817364364</v>
+      </c>
+      <c r="BK68">
+        <v>1171.7750660349864</v>
+      </c>
+      <c r="BM68">
+        <v>0.60439783939940739</v>
+      </c>
+    </row>
+    <row r="69" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>163</v>
+      </c>
+      <c r="B69" t="s">
+        <v>164</v>
+      </c>
+      <c r="C69" s="7">
+        <v>37678</v>
+      </c>
+      <c r="G69">
+        <v>139</v>
+      </c>
+      <c r="H69" t="s">
+        <v>124</v>
+      </c>
+      <c r="I69" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J69" s="14">
+        <v>380</v>
+      </c>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="CM69">
+        <v>463.66798189112399</v>
+      </c>
+      <c r="CO69">
+        <v>26.03107845687958</v>
+      </c>
+      <c r="CQ69">
+        <v>35.961798445284096</v>
+      </c>
+      <c r="CS69">
+        <v>39.829993226858448</v>
+      </c>
+      <c r="CU69">
+        <v>40.488108639754593</v>
+      </c>
+      <c r="CW69">
+        <v>49.624993900759193</v>
+      </c>
+      <c r="CY69">
+        <v>63.449883919386359</v>
+      </c>
+      <c r="DA69">
+        <v>68.975767096205388</v>
+      </c>
+      <c r="DC69">
+        <v>68.650771830577654</v>
+      </c>
+      <c r="DE69">
+        <v>70.655586375418707</v>
+      </c>
+    </row>
+    <row r="70" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>163</v>
+      </c>
+      <c r="B70" t="s">
+        <v>164</v>
+      </c>
+      <c r="C70" s="7">
+        <v>37683</v>
+      </c>
+      <c r="G70">
+        <v>144</v>
+      </c>
+      <c r="H70" t="s">
+        <v>124</v>
+      </c>
+      <c r="I70" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J70" s="14">
+        <v>380</v>
+      </c>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="CM70">
+        <v>445.00739910045422</v>
+      </c>
+      <c r="CO70">
+        <v>24.058702898360281</v>
+      </c>
+      <c r="CQ70">
+        <v>33.137178317668834</v>
+      </c>
+      <c r="CS70">
+        <v>36.393168292845246</v>
+      </c>
+      <c r="CU70">
+        <v>37.367138479523334</v>
+      </c>
+      <c r="CW70">
+        <v>46.752086533120348</v>
+      </c>
+      <c r="CY70">
+        <v>61.663679471190221</v>
+      </c>
+      <c r="DA70">
+        <v>67.44422690693473</v>
+      </c>
+      <c r="DC70">
+        <v>68.232340426081961</v>
+      </c>
+      <c r="DE70">
+        <v>69.95887777472926</v>
+      </c>
+    </row>
+    <row r="71" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>163</v>
+      </c>
+      <c r="B71" t="s">
+        <v>164</v>
+      </c>
+      <c r="C71" s="7">
+        <v>37690</v>
+      </c>
+      <c r="G71">
+        <v>151</v>
+      </c>
+      <c r="H71" t="s">
+        <v>124</v>
+      </c>
+      <c r="I71" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J71" s="14">
+        <v>380</v>
+      </c>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="CM71">
+        <v>422.91337711787162</v>
+      </c>
+      <c r="CO71">
+        <v>22.613849135906971</v>
+      </c>
+      <c r="CQ71">
+        <v>29.253957265661104</v>
+      </c>
+      <c r="CS71">
+        <v>31.029730799782669</v>
+      </c>
+      <c r="CU71">
+        <v>34.216715623344562</v>
+      </c>
+      <c r="CW71">
+        <v>43.639241254529786</v>
+      </c>
+      <c r="CY71">
+        <v>58.978152186389856</v>
+      </c>
+      <c r="DA71">
+        <v>66.664238269428196</v>
+      </c>
+      <c r="DC71">
+        <v>67.38735273544988</v>
+      </c>
+      <c r="DE71">
+        <v>69.130139847378572</v>
+      </c>
+    </row>
+    <row r="72" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>163</v>
+      </c>
+      <c r="B72" t="s">
+        <v>164</v>
+      </c>
+      <c r="C72" s="7">
+        <v>37697</v>
+      </c>
+      <c r="G72" s="13">
+        <v>158</v>
+      </c>
+      <c r="H72" t="s">
+        <v>124</v>
+      </c>
+      <c r="I72" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J72" s="14">
+        <v>380</v>
+      </c>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="AC72">
+        <v>279.40264957031496</v>
+      </c>
+      <c r="AJ72">
+        <v>135.12584023274374</v>
+      </c>
+      <c r="AK72">
+        <v>1.6312750689369722</v>
+      </c>
+      <c r="AQ72">
+        <v>1.2072265868076956E-2</v>
+      </c>
+      <c r="AR72">
+        <v>1.5076837778112202E-2</v>
+      </c>
+      <c r="AS72">
+        <v>2.0372703728201844</v>
+      </c>
+      <c r="BH72">
+        <v>685.17875096619355</v>
+      </c>
+      <c r="BK72">
+        <v>1099.7072407692522</v>
+      </c>
+      <c r="BM72">
+        <v>0.6230555965848753</v>
+      </c>
+    </row>
+    <row r="73" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>163</v>
+      </c>
+      <c r="B73" t="s">
+        <v>164</v>
+      </c>
+      <c r="C73" s="7">
+        <v>37698</v>
+      </c>
+      <c r="G73">
+        <v>159</v>
+      </c>
+      <c r="H73" t="s">
+        <v>124</v>
+      </c>
+      <c r="I73" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J73" s="14">
+        <v>380</v>
+      </c>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="CM73">
+        <v>399.40407529933975</v>
+      </c>
+      <c r="CO73">
+        <v>22.270049346344887</v>
+      </c>
+      <c r="CQ73">
+        <v>27.143324300893848</v>
+      </c>
+      <c r="CS73">
+        <v>26.359955076794279</v>
+      </c>
+      <c r="CU73">
+        <v>29.987714729363773</v>
+      </c>
+      <c r="CW73">
+        <v>38.856986701328047</v>
+      </c>
+      <c r="CY73">
+        <v>55.910501561925649</v>
+      </c>
+      <c r="DA73">
+        <v>64.375052867162893</v>
+      </c>
+      <c r="DC73">
+        <v>65.918780378894596</v>
+      </c>
+      <c r="DE73">
+        <v>68.581710336631772</v>
+      </c>
+    </row>
+    <row r="74" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>163</v>
+      </c>
+      <c r="B74" t="s">
+        <v>164</v>
+      </c>
+      <c r="C74" s="7">
+        <v>37712</v>
+      </c>
+      <c r="G74" s="13">
+        <v>173</v>
+      </c>
+      <c r="H74" t="s">
+        <v>124</v>
+      </c>
+      <c r="I74" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J74" s="14">
+        <v>380</v>
+      </c>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="AC74">
+        <v>341.37321490770455</v>
+      </c>
+      <c r="AJ74">
+        <v>92.741828531482483</v>
+      </c>
+      <c r="AK74">
+        <v>1.0930179610660558</v>
+      </c>
+      <c r="AQ74">
+        <v>1.1785598562950653E-2</v>
+      </c>
+      <c r="AR74">
+        <v>1.756725381973891E-2</v>
+      </c>
+      <c r="AS74">
+        <v>1.6292192415192568</v>
+      </c>
+      <c r="BH74">
+        <v>730.38715588683078</v>
+      </c>
+      <c r="BK74">
+        <v>1164.5021993260179</v>
+      </c>
+      <c r="BM74">
+        <v>0.62720976938434203</v>
+      </c>
+    </row>
+    <row r="75" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>163</v>
+      </c>
+      <c r="B75" t="s">
+        <v>164</v>
+      </c>
+      <c r="C75" s="7">
+        <v>37722</v>
+      </c>
+      <c r="G75" s="14">
+        <v>183</v>
+      </c>
+      <c r="H75" t="s">
+        <v>124</v>
+      </c>
+      <c r="I75" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="J75" s="14">
+        <v>380</v>
+      </c>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="BN75">
+        <v>989.1681890731428</v>
+      </c>
+      <c r="BO75">
+        <v>0.43895467403460303</v>
+      </c>
+      <c r="BP75">
+        <v>434.2</v>
+      </c>
+      <c r="BQ75">
+        <v>532.5</v>
+      </c>
+      <c r="BR75">
+        <v>19.127753303964756</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:ET44" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:ET11">

</xml_diff>

<commit_message>
Corrected Heights and Nodes data UNR treatment
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/Narrabri0203Observed.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/Narrabri0203Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31B81F8-D68E-4ECD-A439-C4679FD1BD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE1EA23-2404-4C2F-82EB-C9DE08B229A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="17640" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -953,7 +953,7 @@
   <dimension ref="A1:ET75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="BV2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
@@ -6230,10 +6230,10 @@
         <v>380</v>
       </c>
       <c r="M49" s="1">
-        <v>285</v>
+        <v>277.75</v>
       </c>
       <c r="N49" s="1">
-        <v>14.166666666666666</v>
+        <v>12.625</v>
       </c>
     </row>
     <row r="50" spans="1:109" x14ac:dyDescent="0.25">
@@ -6259,10 +6259,10 @@
         <v>380</v>
       </c>
       <c r="M50" s="1">
-        <v>356.66666666666663</v>
+        <v>350</v>
       </c>
       <c r="N50" s="1">
-        <v>16.069444444444446</v>
+        <v>14.25</v>
       </c>
       <c r="AC50">
         <v>107.40503651758718</v>
@@ -6370,10 +6370,10 @@
         <v>380</v>
       </c>
       <c r="M52" s="1">
-        <v>456.25</v>
+        <v>456.1875</v>
       </c>
       <c r="N52" s="1">
-        <v>18.041666666666668</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:109" x14ac:dyDescent="0.25">
@@ -6561,10 +6561,10 @@
         <v>380</v>
       </c>
       <c r="M56" s="1">
-        <v>512.5</v>
+        <v>520.875</v>
       </c>
       <c r="N56" s="1">
-        <v>19.652777777777775</v>
+        <v>16.833333333333332</v>
       </c>
     </row>
     <row r="57" spans="1:109" x14ac:dyDescent="0.25">
@@ -6697,10 +6697,10 @@
         <v>380</v>
       </c>
       <c r="M59" s="1">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="N59" s="1">
-        <v>21.027777777777775</v>
+        <v>17.75</v>
       </c>
     </row>
     <row r="60" spans="1:109" x14ac:dyDescent="0.25">
@@ -6726,10 +6726,10 @@
         <v>380</v>
       </c>
       <c r="M60" s="1">
-        <v>554.58333333333337</v>
+        <v>566.4375</v>
       </c>
       <c r="N60" s="1">
-        <v>21.375</v>
+        <v>18.166666666666668</v>
       </c>
       <c r="AC60">
         <v>255.3324384499268</v>
@@ -6837,10 +6837,10 @@
         <v>380</v>
       </c>
       <c r="M62" s="1">
-        <v>561.25</v>
+        <v>573.4375</v>
       </c>
       <c r="N62" s="1">
-        <v>21.625</v>
+        <v>18.291666666666668</v>
       </c>
     </row>
     <row r="63" spans="1:109" x14ac:dyDescent="0.25">
@@ -6973,10 +6973,10 @@
         <v>380</v>
       </c>
       <c r="M65" s="1">
-        <v>561.25</v>
+        <v>573.9375</v>
       </c>
       <c r="N65" s="1">
-        <v>21.833333333333332</v>
+        <v>18.375</v>
       </c>
     </row>
     <row r="66" spans="1:109" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added phenology data to UNR treatment Narrabri0203 test set
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/Narrabri0203Observed.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/Narrabri0203Observed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408A2060-A54C-447D-B187-57C5F8DACD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68240624-217B-407E-8510-D4EA4915FDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2CD5F283-94FE-4198-B98E-779709417693}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="159">
   <si>
     <t>SimulationName</t>
   </si>
@@ -593,7 +593,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -612,6 +612,9 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -930,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C911DF83-7300-4B7A-8A42-16858D40307A}">
-  <dimension ref="A1:EL75"/>
+  <dimension ref="A1:EL77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
@@ -5475,6 +5478,12 @@
       <c r="C47" s="7">
         <v>37599</v>
       </c>
+      <c r="D47" s="1">
+        <v>4</v>
+      </c>
+      <c r="E47" t="s">
+        <v>62</v>
+      </c>
       <c r="F47">
         <v>60</v>
       </c>
@@ -5750,10 +5759,16 @@
         <v>146</v>
       </c>
       <c r="C52" s="7">
-        <v>37620</v>
-      </c>
-      <c r="F52">
-        <v>81</v>
+        <v>37618</v>
+      </c>
+      <c r="D52" s="1">
+        <v>5</v>
+      </c>
+      <c r="E52" t="s">
+        <v>59</v>
+      </c>
+      <c r="F52" s="16">
+        <v>79</v>
       </c>
       <c r="G52" t="s">
         <v>106</v>
@@ -5764,12 +5779,8 @@
       <c r="I52" s="14">
         <v>380</v>
       </c>
-      <c r="L52" s="1">
-        <v>456.1875</v>
-      </c>
-      <c r="M52" s="1">
-        <v>16</v>
-      </c>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
     </row>
     <row r="53" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -5779,10 +5790,10 @@
         <v>146</v>
       </c>
       <c r="C53" s="7">
-        <v>37621</v>
+        <v>37620</v>
       </c>
       <c r="F53">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G53" t="s">
         <v>106</v>
@@ -5793,37 +5804,11 @@
       <c r="I53" s="14">
         <v>380</v>
       </c>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="CE53">
-        <v>408.87650658986809</v>
-      </c>
-      <c r="CG53">
-        <v>23.006534955025746</v>
-      </c>
-      <c r="CI53">
-        <v>28.28750421328056</v>
-      </c>
-      <c r="CK53">
-        <v>30.578118238717931</v>
-      </c>
-      <c r="CM53">
-        <v>31.539223970133133</v>
-      </c>
-      <c r="CO53">
-        <v>40.015934340142039</v>
-      </c>
-      <c r="CQ53">
-        <v>57.18367079470331</v>
-      </c>
-      <c r="CS53">
-        <v>66.481299017251601</v>
-      </c>
-      <c r="CU53">
-        <v>65.845461116481573</v>
-      </c>
-      <c r="CW53">
-        <v>65.938759944132258</v>
+      <c r="L53" s="1">
+        <v>456.1875</v>
+      </c>
+      <c r="M53" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:101" x14ac:dyDescent="0.25">
@@ -5834,10 +5819,10 @@
         <v>146</v>
       </c>
       <c r="C54" s="7">
-        <v>37623</v>
-      </c>
-      <c r="F54" s="12">
-        <v>84</v>
+        <v>37621</v>
+      </c>
+      <c r="F54">
+        <v>82</v>
       </c>
       <c r="G54" t="s">
         <v>106</v>
@@ -5850,32 +5835,35 @@
       </c>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
-      <c r="U54">
-        <v>163.05283592784707</v>
-      </c>
-      <c r="AB54">
-        <v>154.2014351487644</v>
-      </c>
-      <c r="AC54">
-        <v>2.0754754761103751</v>
-      </c>
-      <c r="AI54">
-        <v>1.345950816935056E-2</v>
-      </c>
-      <c r="AJ54">
-        <v>3.1896323007026821E-2</v>
-      </c>
-      <c r="AK54">
-        <v>4.9184587836520883</v>
-      </c>
-      <c r="AZ54">
-        <v>51.020777672873862</v>
-      </c>
-      <c r="BC54">
-        <v>368.27504874948534</v>
-      </c>
-      <c r="BE54">
-        <v>0.13853987080069638</v>
+      <c r="CE54">
+        <v>408.87650658986809</v>
+      </c>
+      <c r="CG54">
+        <v>23.006534955025746</v>
+      </c>
+      <c r="CI54">
+        <v>28.28750421328056</v>
+      </c>
+      <c r="CK54">
+        <v>30.578118238717931</v>
+      </c>
+      <c r="CM54">
+        <v>31.539223970133133</v>
+      </c>
+      <c r="CO54">
+        <v>40.015934340142039</v>
+      </c>
+      <c r="CQ54">
+        <v>57.18367079470331</v>
+      </c>
+      <c r="CS54">
+        <v>66.481299017251601</v>
+      </c>
+      <c r="CU54">
+        <v>65.845461116481573</v>
+      </c>
+      <c r="CW54">
+        <v>65.938759944132258</v>
       </c>
     </row>
     <row r="55" spans="1:101" x14ac:dyDescent="0.25">
@@ -5886,10 +5874,10 @@
         <v>146</v>
       </c>
       <c r="C55" s="7">
-        <v>37627</v>
-      </c>
-      <c r="F55">
-        <v>88</v>
+        <v>37623</v>
+      </c>
+      <c r="F55" s="12">
+        <v>84</v>
       </c>
       <c r="G55" t="s">
         <v>106</v>
@@ -5902,35 +5890,32 @@
       </c>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
-      <c r="CE55">
-        <v>475.48820047784938</v>
-      </c>
-      <c r="CG55">
-        <v>25.719230320622518</v>
-      </c>
-      <c r="CI55">
-        <v>34.918861782779999</v>
-      </c>
-      <c r="CK55">
-        <v>39.021567503609475</v>
-      </c>
-      <c r="CM55">
-        <v>39.832024447268623</v>
-      </c>
-      <c r="CO55">
-        <v>49.032131443539868</v>
-      </c>
-      <c r="CQ55">
-        <v>66.832119804876172</v>
-      </c>
-      <c r="CS55">
-        <v>75.28880013102399</v>
-      </c>
-      <c r="CU55">
-        <v>72.835085875534631</v>
-      </c>
-      <c r="CW55">
-        <v>72.008379168594118</v>
+      <c r="U55">
+        <v>163.05283592784707</v>
+      </c>
+      <c r="AB55">
+        <v>154.2014351487644</v>
+      </c>
+      <c r="AC55">
+        <v>2.0754754761103751</v>
+      </c>
+      <c r="AI55">
+        <v>1.345950816935056E-2</v>
+      </c>
+      <c r="AJ55">
+        <v>3.1896323007026821E-2</v>
+      </c>
+      <c r="AK55">
+        <v>4.9184587836520883</v>
+      </c>
+      <c r="AZ55">
+        <v>51.020777672873862</v>
+      </c>
+      <c r="BC55">
+        <v>368.27504874948534</v>
+      </c>
+      <c r="BE55">
+        <v>0.13853987080069638</v>
       </c>
     </row>
     <row r="56" spans="1:101" x14ac:dyDescent="0.25">
@@ -5941,10 +5926,10 @@
         <v>146</v>
       </c>
       <c r="C56" s="7">
-        <v>37628</v>
+        <v>37627</v>
       </c>
       <c r="F56">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G56" t="s">
         <v>106</v>
@@ -5955,11 +5940,37 @@
       <c r="I56" s="14">
         <v>380</v>
       </c>
-      <c r="L56" s="1">
-        <v>520.875</v>
-      </c>
-      <c r="M56" s="1">
-        <v>16.833333333333332</v>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="CE56">
+        <v>475.48820047784938</v>
+      </c>
+      <c r="CG56">
+        <v>25.719230320622518</v>
+      </c>
+      <c r="CI56">
+        <v>34.918861782779999</v>
+      </c>
+      <c r="CK56">
+        <v>39.021567503609475</v>
+      </c>
+      <c r="CM56">
+        <v>39.832024447268623</v>
+      </c>
+      <c r="CO56">
+        <v>49.032131443539868</v>
+      </c>
+      <c r="CQ56">
+        <v>66.832119804876172</v>
+      </c>
+      <c r="CS56">
+        <v>75.28880013102399</v>
+      </c>
+      <c r="CU56">
+        <v>72.835085875534631</v>
+      </c>
+      <c r="CW56">
+        <v>72.008379168594118</v>
       </c>
     </row>
     <row r="57" spans="1:101" x14ac:dyDescent="0.25">
@@ -5970,10 +5981,10 @@
         <v>146</v>
       </c>
       <c r="C57" s="7">
-        <v>37631</v>
-      </c>
-      <c r="F57" s="12">
-        <v>92</v>
+        <v>37628</v>
+      </c>
+      <c r="F57">
+        <v>89</v>
       </c>
       <c r="G57" t="s">
         <v>106</v>
@@ -5984,34 +5995,11 @@
       <c r="I57" s="14">
         <v>380</v>
       </c>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-      <c r="U57">
-        <v>234.79999999999998</v>
-      </c>
-      <c r="AB57">
-        <v>187.80000000000004</v>
-      </c>
-      <c r="AC57">
-        <v>2.7587953333333335</v>
-      </c>
-      <c r="AI57">
-        <v>1.4690070997515084E-2</v>
-      </c>
-      <c r="AJ57">
-        <v>2.9367473950285786E-2</v>
-      </c>
-      <c r="AK57">
-        <v>5.5152116078636721</v>
-      </c>
-      <c r="AZ57">
-        <v>108.8</v>
-      </c>
-      <c r="BC57">
-        <v>531.4</v>
-      </c>
-      <c r="BE57">
-        <v>0.20474219044034625</v>
+      <c r="L57" s="1">
+        <v>520.875</v>
+      </c>
+      <c r="M57" s="1">
+        <v>16.833333333333332</v>
       </c>
     </row>
     <row r="58" spans="1:101" x14ac:dyDescent="0.25">
@@ -6022,10 +6010,10 @@
         <v>146</v>
       </c>
       <c r="C58" s="7">
-        <v>37634</v>
-      </c>
-      <c r="F58">
-        <v>95</v>
+        <v>37631</v>
+      </c>
+      <c r="F58" s="12">
+        <v>92</v>
       </c>
       <c r="G58" t="s">
         <v>106</v>
@@ -6038,35 +6026,32 @@
       </c>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
-      <c r="CE58">
-        <v>436.11211502542864</v>
-      </c>
-      <c r="CG58">
-        <v>23.226042813231285</v>
-      </c>
-      <c r="CI58">
-        <v>29.185236632860441</v>
-      </c>
-      <c r="CK58">
-        <v>29.839435639421122</v>
-      </c>
-      <c r="CM58">
-        <v>33.329072304098837</v>
-      </c>
-      <c r="CO58">
-        <v>42.237699171510215</v>
-      </c>
-      <c r="CQ58">
-        <v>61.29044272082087</v>
-      </c>
-      <c r="CS58">
-        <v>71.575729221227206</v>
-      </c>
-      <c r="CU58">
-        <v>72.394311046527037</v>
-      </c>
-      <c r="CW58">
-        <v>73.034145475731634</v>
+      <c r="U58">
+        <v>234.79999999999998</v>
+      </c>
+      <c r="AB58">
+        <v>187.80000000000004</v>
+      </c>
+      <c r="AC58">
+        <v>2.7587953333333335</v>
+      </c>
+      <c r="AI58">
+        <v>1.4690070997515084E-2</v>
+      </c>
+      <c r="AJ58">
+        <v>2.9367473950285786E-2</v>
+      </c>
+      <c r="AK58">
+        <v>5.5152116078636721</v>
+      </c>
+      <c r="AZ58">
+        <v>108.8</v>
+      </c>
+      <c r="BC58">
+        <v>531.4</v>
+      </c>
+      <c r="BE58">
+        <v>0.20474219044034625</v>
       </c>
     </row>
     <row r="59" spans="1:101" x14ac:dyDescent="0.25">
@@ -6077,10 +6062,10 @@
         <v>146</v>
       </c>
       <c r="C59" s="7">
-        <v>37636</v>
+        <v>37634</v>
       </c>
       <c r="F59">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G59" t="s">
         <v>106</v>
@@ -6091,11 +6076,37 @@
       <c r="I59" s="14">
         <v>380</v>
       </c>
-      <c r="L59" s="1">
-        <v>561</v>
-      </c>
-      <c r="M59" s="1">
-        <v>17.75</v>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="CE59">
+        <v>436.11211502542864</v>
+      </c>
+      <c r="CG59">
+        <v>23.226042813231285</v>
+      </c>
+      <c r="CI59">
+        <v>29.185236632860441</v>
+      </c>
+      <c r="CK59">
+        <v>29.839435639421122</v>
+      </c>
+      <c r="CM59">
+        <v>33.329072304098837</v>
+      </c>
+      <c r="CO59">
+        <v>42.237699171510215</v>
+      </c>
+      <c r="CQ59">
+        <v>61.29044272082087</v>
+      </c>
+      <c r="CS59">
+        <v>71.575729221227206</v>
+      </c>
+      <c r="CU59">
+        <v>72.394311046527037</v>
+      </c>
+      <c r="CW59">
+        <v>73.034145475731634</v>
       </c>
     </row>
     <row r="60" spans="1:101" x14ac:dyDescent="0.25">
@@ -6106,10 +6117,10 @@
         <v>146</v>
       </c>
       <c r="C60" s="7">
-        <v>37642</v>
-      </c>
-      <c r="F60" s="13">
-        <v>103</v>
+        <v>37636</v>
+      </c>
+      <c r="F60">
+        <v>97</v>
       </c>
       <c r="G60" t="s">
         <v>106</v>
@@ -6121,37 +6132,10 @@
         <v>380</v>
       </c>
       <c r="L60" s="1">
-        <v>566.4375</v>
+        <v>561</v>
       </c>
       <c r="M60" s="1">
-        <v>18.166666666666668</v>
-      </c>
-      <c r="U60">
-        <v>255.3324384499268</v>
-      </c>
-      <c r="AB60">
-        <v>172.24948076140012</v>
-      </c>
-      <c r="AC60">
-        <v>2.4590574584663005</v>
-      </c>
-      <c r="AI60">
-        <v>1.4276138584548684E-2</v>
-      </c>
-      <c r="AJ60">
-        <v>2.9680706028275522E-2</v>
-      </c>
-      <c r="AK60">
-        <v>5.1124862020022173</v>
-      </c>
-      <c r="AZ60">
-        <v>309.92831170209831</v>
-      </c>
-      <c r="BC60">
-        <v>737.51023091342518</v>
-      </c>
-      <c r="BE60">
-        <v>0.42023594888744015</v>
+        <v>17.75</v>
       </c>
     </row>
     <row r="61" spans="1:101" x14ac:dyDescent="0.25">
@@ -6162,10 +6146,10 @@
         <v>146</v>
       </c>
       <c r="C61" s="7">
-        <v>37645</v>
-      </c>
-      <c r="F61">
-        <v>106</v>
+        <v>37642</v>
+      </c>
+      <c r="F61" s="13">
+        <v>103</v>
       </c>
       <c r="G61" t="s">
         <v>106</v>
@@ -6176,37 +6160,38 @@
       <c r="I61" s="14">
         <v>380</v>
       </c>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="CE61">
-        <v>443.730802273839</v>
-      </c>
-      <c r="CG61">
-        <v>23.958374706982497</v>
-      </c>
-      <c r="CI61">
-        <v>30.718818401610406</v>
-      </c>
-      <c r="CK61">
-        <v>32.833454524016553</v>
-      </c>
-      <c r="CM61">
-        <v>35.591851841031882</v>
-      </c>
-      <c r="CO61">
-        <v>44.534247747762386</v>
-      </c>
-      <c r="CQ61">
-        <v>61.494834274594574</v>
-      </c>
-      <c r="CS61">
-        <v>71.25479639641982</v>
-      </c>
-      <c r="CU61">
-        <v>71.923067911366829</v>
-      </c>
-      <c r="CW61">
-        <v>71.421356470054036</v>
+      <c r="L61" s="1">
+        <v>566.4375</v>
+      </c>
+      <c r="M61" s="1">
+        <v>18.166666666666668</v>
+      </c>
+      <c r="U61">
+        <v>255.3324384499268</v>
+      </c>
+      <c r="AB61">
+        <v>172.24948076140012</v>
+      </c>
+      <c r="AC61">
+        <v>2.4590574584663005</v>
+      </c>
+      <c r="AI61">
+        <v>1.4276138584548684E-2</v>
+      </c>
+      <c r="AJ61">
+        <v>2.9680706028275522E-2</v>
+      </c>
+      <c r="AK61">
+        <v>5.1124862020022173</v>
+      </c>
+      <c r="AZ61">
+        <v>309.92831170209831</v>
+      </c>
+      <c r="BC61">
+        <v>737.51023091342518</v>
+      </c>
+      <c r="BE61">
+        <v>0.42023594888744015</v>
       </c>
     </row>
     <row r="62" spans="1:101" x14ac:dyDescent="0.25">
@@ -6217,10 +6202,10 @@
         <v>146</v>
       </c>
       <c r="C62" s="7">
-        <v>37650</v>
+        <v>37645</v>
       </c>
       <c r="F62">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G62" t="s">
         <v>106</v>
@@ -6231,11 +6216,37 @@
       <c r="I62" s="14">
         <v>380</v>
       </c>
-      <c r="L62" s="1">
-        <v>573.4375</v>
-      </c>
-      <c r="M62" s="1">
-        <v>18.291666666666668</v>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="CE62">
+        <v>443.730802273839</v>
+      </c>
+      <c r="CG62">
+        <v>23.958374706982497</v>
+      </c>
+      <c r="CI62">
+        <v>30.718818401610406</v>
+      </c>
+      <c r="CK62">
+        <v>32.833454524016553</v>
+      </c>
+      <c r="CM62">
+        <v>35.591851841031882</v>
+      </c>
+      <c r="CO62">
+        <v>44.534247747762386</v>
+      </c>
+      <c r="CQ62">
+        <v>61.494834274594574</v>
+      </c>
+      <c r="CS62">
+        <v>71.25479639641982</v>
+      </c>
+      <c r="CU62">
+        <v>71.923067911366829</v>
+      </c>
+      <c r="CW62">
+        <v>71.421356470054036</v>
       </c>
     </row>
     <row r="63" spans="1:101" x14ac:dyDescent="0.25">
@@ -6246,10 +6257,10 @@
         <v>146</v>
       </c>
       <c r="C63" s="7">
-        <v>37652</v>
-      </c>
-      <c r="F63" s="13">
-        <v>113</v>
+        <v>37650</v>
+      </c>
+      <c r="F63">
+        <v>111</v>
       </c>
       <c r="G63" t="s">
         <v>106</v>
@@ -6260,34 +6271,11 @@
       <c r="I63" s="14">
         <v>380</v>
       </c>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-      <c r="U63">
-        <v>268.98330719342749</v>
-      </c>
-      <c r="AB63">
-        <v>173.42593278609607</v>
-      </c>
-      <c r="AC63">
-        <v>2.6444006755744387</v>
-      </c>
-      <c r="AI63">
-        <v>1.5248011834747046E-2</v>
-      </c>
-      <c r="AJ63">
-        <v>2.2503378117184086E-2</v>
-      </c>
-      <c r="AK63">
-        <v>3.9026693408108724</v>
-      </c>
-      <c r="AZ63">
-        <v>456.71547635604867</v>
-      </c>
-      <c r="BC63">
-        <v>899.1247163355722</v>
-      </c>
-      <c r="BE63">
-        <v>0.50795564626163925</v>
+      <c r="L63" s="1">
+        <v>573.4375</v>
+      </c>
+      <c r="M63" s="1">
+        <v>18.291666666666668</v>
       </c>
     </row>
     <row r="64" spans="1:101" x14ac:dyDescent="0.25">
@@ -6298,10 +6286,10 @@
         <v>146</v>
       </c>
       <c r="C64" s="7">
-        <v>37655</v>
-      </c>
-      <c r="F64">
-        <v>116</v>
+        <v>37652</v>
+      </c>
+      <c r="F64" s="13">
+        <v>113</v>
       </c>
       <c r="G64" t="s">
         <v>106</v>
@@ -6314,35 +6302,32 @@
       </c>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
-      <c r="CE64">
-        <v>461.56463903673188</v>
-      </c>
-      <c r="CG64">
-        <v>24.451069200946005</v>
-      </c>
-      <c r="CI64">
-        <v>33.256934126299399</v>
-      </c>
-      <c r="CK64">
-        <v>37.058392977176993</v>
-      </c>
-      <c r="CM64">
-        <v>38.230407153846983</v>
-      </c>
-      <c r="CO64">
-        <v>47.890839475573756</v>
-      </c>
-      <c r="CQ64">
-        <v>65.088570985293643</v>
-      </c>
-      <c r="CS64">
-        <v>72.516184271137433</v>
-      </c>
-      <c r="CU64">
-        <v>71.502605286460962</v>
-      </c>
-      <c r="CW64">
-        <v>71.569635559996684</v>
+      <c r="U64">
+        <v>268.98330719342749</v>
+      </c>
+      <c r="AB64">
+        <v>173.42593278609607</v>
+      </c>
+      <c r="AC64">
+        <v>2.6444006755744387</v>
+      </c>
+      <c r="AI64">
+        <v>1.5248011834747046E-2</v>
+      </c>
+      <c r="AJ64">
+        <v>2.2503378117184086E-2</v>
+      </c>
+      <c r="AK64">
+        <v>3.9026693408108724</v>
+      </c>
+      <c r="AZ64">
+        <v>456.71547635604867</v>
+      </c>
+      <c r="BC64">
+        <v>899.1247163355722</v>
+      </c>
+      <c r="BE64">
+        <v>0.50795564626163925</v>
       </c>
     </row>
     <row r="65" spans="1:101" x14ac:dyDescent="0.25">
@@ -6353,10 +6338,10 @@
         <v>146</v>
       </c>
       <c r="C65" s="7">
-        <v>37657</v>
+        <v>37655</v>
       </c>
       <c r="F65">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G65" t="s">
         <v>106</v>
@@ -6367,11 +6352,37 @@
       <c r="I65" s="14">
         <v>380</v>
       </c>
-      <c r="L65" s="1">
-        <v>573.9375</v>
-      </c>
-      <c r="M65" s="1">
-        <v>18.375</v>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="CE65">
+        <v>461.56463903673188</v>
+      </c>
+      <c r="CG65">
+        <v>24.451069200946005</v>
+      </c>
+      <c r="CI65">
+        <v>33.256934126299399</v>
+      </c>
+      <c r="CK65">
+        <v>37.058392977176993</v>
+      </c>
+      <c r="CM65">
+        <v>38.230407153846983</v>
+      </c>
+      <c r="CO65">
+        <v>47.890839475573756</v>
+      </c>
+      <c r="CQ65">
+        <v>65.088570985293643</v>
+      </c>
+      <c r="CS65">
+        <v>72.516184271137433</v>
+      </c>
+      <c r="CU65">
+        <v>71.502605286460962</v>
+      </c>
+      <c r="CW65">
+        <v>71.569635559996684</v>
       </c>
     </row>
     <row r="66" spans="1:101" x14ac:dyDescent="0.25">
@@ -6382,10 +6393,10 @@
         <v>146</v>
       </c>
       <c r="C66" s="7">
-        <v>37662</v>
-      </c>
-      <c r="F66" s="13">
-        <v>123</v>
+        <v>37657</v>
+      </c>
+      <c r="F66">
+        <v>118</v>
       </c>
       <c r="G66" t="s">
         <v>106</v>
@@ -6396,64 +6407,11 @@
       <c r="I66" s="14">
         <v>380</v>
       </c>
-      <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
-      <c r="U66">
-        <v>253.15990812250848</v>
-      </c>
-      <c r="AB66">
-        <v>177.13490031457911</v>
-      </c>
-      <c r="AC66">
-        <v>2.6083667777078143</v>
-      </c>
-      <c r="AI66">
-        <v>1.4725312589870988E-2</v>
-      </c>
-      <c r="AJ66">
-        <v>1.8026579901579902E-2</v>
-      </c>
-      <c r="AK66">
-        <v>3.1931364338791512</v>
-      </c>
-      <c r="AZ66">
-        <v>628.03692962352477</v>
-      </c>
-      <c r="BC66">
-        <v>1058.3317380606122</v>
-      </c>
-      <c r="BE66">
-        <v>0.59342161539480942</v>
-      </c>
-      <c r="CE66">
-        <v>421.00743659410091</v>
-      </c>
-      <c r="CG66">
-        <v>23.317744058216707</v>
-      </c>
-      <c r="CI66">
-        <v>29.504080157104671</v>
-      </c>
-      <c r="CK66">
-        <v>30.357396844015312</v>
-      </c>
-      <c r="CM66">
-        <v>32.72173740145702</v>
-      </c>
-      <c r="CO66">
-        <v>41.507729336604193</v>
-      </c>
-      <c r="CQ66">
-        <v>57.636277202919132</v>
-      </c>
-      <c r="CS66">
-        <v>66.690644134760433</v>
-      </c>
-      <c r="CU66">
-        <v>68.370463413973752</v>
-      </c>
-      <c r="CW66">
-        <v>70.901364045049675</v>
+      <c r="L66" s="1">
+        <v>573.9375</v>
+      </c>
+      <c r="M66" s="1">
+        <v>18.375</v>
       </c>
     </row>
     <row r="67" spans="1:101" x14ac:dyDescent="0.25">
@@ -6464,10 +6422,10 @@
         <v>146</v>
       </c>
       <c r="C67" s="7">
-        <v>37670</v>
-      </c>
-      <c r="F67">
-        <v>131</v>
+        <v>37662</v>
+      </c>
+      <c r="F67" s="13">
+        <v>123</v>
       </c>
       <c r="G67" t="s">
         <v>106</v>
@@ -6480,35 +6438,62 @@
       </c>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
+      <c r="U67">
+        <v>253.15990812250848</v>
+      </c>
+      <c r="AB67">
+        <v>177.13490031457911</v>
+      </c>
+      <c r="AC67">
+        <v>2.6083667777078143</v>
+      </c>
+      <c r="AI67">
+        <v>1.4725312589870988E-2</v>
+      </c>
+      <c r="AJ67">
+        <v>1.8026579901579902E-2</v>
+      </c>
+      <c r="AK67">
+        <v>3.1931364338791512</v>
+      </c>
+      <c r="AZ67">
+        <v>628.03692962352477</v>
+      </c>
+      <c r="BC67">
+        <v>1058.3317380606122</v>
+      </c>
+      <c r="BE67">
+        <v>0.59342161539480942</v>
+      </c>
       <c r="CE67">
-        <v>464.52009603585321</v>
+        <v>421.00743659410091</v>
       </c>
       <c r="CG67">
-        <v>25.277338955413999</v>
+        <v>23.317744058216707</v>
       </c>
       <c r="CI67">
-        <v>34.64701104420093</v>
+        <v>29.504080157104671</v>
       </c>
       <c r="CK67">
-        <v>38.235485204872425</v>
+        <v>30.357396844015312</v>
       </c>
       <c r="CM67">
-        <v>39.662417543019153</v>
+        <v>32.72173740145702</v>
       </c>
       <c r="CO67">
-        <v>47.909882166919125</v>
+        <v>41.507729336604193</v>
       </c>
       <c r="CQ67">
-        <v>65.131226613907302</v>
+        <v>57.636277202919132</v>
       </c>
       <c r="CS67">
-        <v>72.181032903458842</v>
+        <v>66.690644134760433</v>
       </c>
       <c r="CU67">
-        <v>70.206686664770416</v>
+        <v>68.370463413973752</v>
       </c>
       <c r="CW67">
-        <v>71.26901493929104</v>
+        <v>70.901364045049675</v>
       </c>
     </row>
     <row r="68" spans="1:101" x14ac:dyDescent="0.25">
@@ -6519,10 +6504,10 @@
         <v>146</v>
       </c>
       <c r="C68" s="7">
-        <v>37677</v>
-      </c>
-      <c r="F68" s="13">
-        <v>138</v>
+        <v>37670</v>
+      </c>
+      <c r="F68">
+        <v>131</v>
       </c>
       <c r="G68" t="s">
         <v>106</v>
@@ -6535,32 +6520,35 @@
       </c>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
-      <c r="U68">
-        <v>272.7232065679861</v>
-      </c>
-      <c r="AB68">
-        <v>190.83354129335666</v>
-      </c>
-      <c r="AC68">
-        <v>2.4936474491697287</v>
-      </c>
-      <c r="AI68">
-        <v>1.3067133965388181E-2</v>
-      </c>
-      <c r="AJ68">
-        <v>1.4813365831153892E-2</v>
-      </c>
-      <c r="AK68">
-        <v>2.8268870600331049</v>
-      </c>
-      <c r="AZ68">
-        <v>708.21831817364364</v>
-      </c>
-      <c r="BC68">
-        <v>1171.7750660349864</v>
-      </c>
-      <c r="BE68">
-        <v>0.60439783939940739</v>
+      <c r="CE68">
+        <v>464.52009603585321</v>
+      </c>
+      <c r="CG68">
+        <v>25.277338955413999</v>
+      </c>
+      <c r="CI68">
+        <v>34.64701104420093</v>
+      </c>
+      <c r="CK68">
+        <v>38.235485204872425</v>
+      </c>
+      <c r="CM68">
+        <v>39.662417543019153</v>
+      </c>
+      <c r="CO68">
+        <v>47.909882166919125</v>
+      </c>
+      <c r="CQ68">
+        <v>65.131226613907302</v>
+      </c>
+      <c r="CS68">
+        <v>72.181032903458842</v>
+      </c>
+      <c r="CU68">
+        <v>70.206686664770416</v>
+      </c>
+      <c r="CW68">
+        <v>71.26901493929104</v>
       </c>
     </row>
     <row r="69" spans="1:101" x14ac:dyDescent="0.25">
@@ -6571,10 +6559,10 @@
         <v>146</v>
       </c>
       <c r="C69" s="7">
-        <v>37678</v>
-      </c>
-      <c r="F69">
-        <v>139</v>
+        <v>37677</v>
+      </c>
+      <c r="F69" s="13">
+        <v>138</v>
       </c>
       <c r="G69" t="s">
         <v>106</v>
@@ -6587,35 +6575,32 @@
       </c>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
-      <c r="CE69">
-        <v>463.66798189112399</v>
-      </c>
-      <c r="CG69">
-        <v>26.03107845687958</v>
-      </c>
-      <c r="CI69">
-        <v>35.961798445284096</v>
-      </c>
-      <c r="CK69">
-        <v>39.829993226858448</v>
-      </c>
-      <c r="CM69">
-        <v>40.488108639754593</v>
-      </c>
-      <c r="CO69">
-        <v>49.624993900759193</v>
-      </c>
-      <c r="CQ69">
-        <v>63.449883919386359</v>
-      </c>
-      <c r="CS69">
-        <v>68.975767096205388</v>
-      </c>
-      <c r="CU69">
-        <v>68.650771830577654</v>
-      </c>
-      <c r="CW69">
-        <v>70.655586375418707</v>
+      <c r="U69">
+        <v>272.7232065679861</v>
+      </c>
+      <c r="AB69">
+        <v>190.83354129335666</v>
+      </c>
+      <c r="AC69">
+        <v>2.4936474491697287</v>
+      </c>
+      <c r="AI69">
+        <v>1.3067133965388181E-2</v>
+      </c>
+      <c r="AJ69">
+        <v>1.4813365831153892E-2</v>
+      </c>
+      <c r="AK69">
+        <v>2.8268870600331049</v>
+      </c>
+      <c r="AZ69">
+        <v>708.21831817364364</v>
+      </c>
+      <c r="BC69">
+        <v>1171.7750660349864</v>
+      </c>
+      <c r="BE69">
+        <v>0.60439783939940739</v>
       </c>
     </row>
     <row r="70" spans="1:101" x14ac:dyDescent="0.25">
@@ -6626,10 +6611,10 @@
         <v>146</v>
       </c>
       <c r="C70" s="7">
-        <v>37683</v>
+        <v>37678</v>
       </c>
       <c r="F70">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G70" t="s">
         <v>106</v>
@@ -6643,34 +6628,34 @@
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
       <c r="CE70">
-        <v>445.00739910045422</v>
+        <v>463.66798189112399</v>
       </c>
       <c r="CG70">
-        <v>24.058702898360281</v>
+        <v>26.03107845687958</v>
       </c>
       <c r="CI70">
-        <v>33.137178317668834</v>
+        <v>35.961798445284096</v>
       </c>
       <c r="CK70">
-        <v>36.393168292845246</v>
+        <v>39.829993226858448</v>
       </c>
       <c r="CM70">
-        <v>37.367138479523334</v>
+        <v>40.488108639754593</v>
       </c>
       <c r="CO70">
-        <v>46.752086533120348</v>
+        <v>49.624993900759193</v>
       </c>
       <c r="CQ70">
-        <v>61.663679471190221</v>
+        <v>63.449883919386359</v>
       </c>
       <c r="CS70">
-        <v>67.44422690693473</v>
+        <v>68.975767096205388</v>
       </c>
       <c r="CU70">
-        <v>68.232340426081961</v>
+        <v>68.650771830577654</v>
       </c>
       <c r="CW70">
-        <v>69.95887777472926</v>
+        <v>70.655586375418707</v>
       </c>
     </row>
     <row r="71" spans="1:101" x14ac:dyDescent="0.25">
@@ -6681,10 +6666,10 @@
         <v>146</v>
       </c>
       <c r="C71" s="7">
-        <v>37690</v>
+        <v>37683</v>
       </c>
       <c r="F71">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="G71" t="s">
         <v>106</v>
@@ -6698,34 +6683,34 @@
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
       <c r="CE71">
-        <v>422.91337711787162</v>
+        <v>445.00739910045422</v>
       </c>
       <c r="CG71">
-        <v>22.613849135906971</v>
+        <v>24.058702898360281</v>
       </c>
       <c r="CI71">
-        <v>29.253957265661104</v>
+        <v>33.137178317668834</v>
       </c>
       <c r="CK71">
-        <v>31.029730799782669</v>
+        <v>36.393168292845246</v>
       </c>
       <c r="CM71">
-        <v>34.216715623344562</v>
+        <v>37.367138479523334</v>
       </c>
       <c r="CO71">
-        <v>43.639241254529786</v>
+        <v>46.752086533120348</v>
       </c>
       <c r="CQ71">
-        <v>58.978152186389856</v>
+        <v>61.663679471190221</v>
       </c>
       <c r="CS71">
-        <v>66.664238269428196</v>
+        <v>67.44422690693473</v>
       </c>
       <c r="CU71">
-        <v>67.38735273544988</v>
+        <v>68.232340426081961</v>
       </c>
       <c r="CW71">
-        <v>69.130139847378572</v>
+        <v>69.95887777472926</v>
       </c>
     </row>
     <row r="72" spans="1:101" x14ac:dyDescent="0.25">
@@ -6736,10 +6721,16 @@
         <v>146</v>
       </c>
       <c r="C72" s="7">
-        <v>37697</v>
-      </c>
-      <c r="F72" s="13">
-        <v>158</v>
+        <v>37685</v>
+      </c>
+      <c r="D72" s="1">
+        <v>8</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F72">
+        <v>146</v>
       </c>
       <c r="G72" t="s">
         <v>106</v>
@@ -6752,33 +6743,6 @@
       </c>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
-      <c r="U72">
-        <v>279.40264957031496</v>
-      </c>
-      <c r="AB72">
-        <v>135.12584023274374</v>
-      </c>
-      <c r="AC72">
-        <v>1.6312750689369722</v>
-      </c>
-      <c r="AI72">
-        <v>1.2072265868076956E-2</v>
-      </c>
-      <c r="AJ72">
-        <v>1.5076837778112202E-2</v>
-      </c>
-      <c r="AK72">
-        <v>2.0372703728201844</v>
-      </c>
-      <c r="AZ72">
-        <v>685.17875096619355</v>
-      </c>
-      <c r="BC72">
-        <v>1099.7072407692522</v>
-      </c>
-      <c r="BE72">
-        <v>0.6230555965848753</v>
-      </c>
     </row>
     <row r="73" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
@@ -6788,10 +6752,10 @@
         <v>146</v>
       </c>
       <c r="C73" s="7">
-        <v>37698</v>
+        <v>37690</v>
       </c>
       <c r="F73">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="G73" t="s">
         <v>106</v>
@@ -6805,34 +6769,34 @@
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
       <c r="CE73">
-        <v>399.40407529933975</v>
+        <v>422.91337711787162</v>
       </c>
       <c r="CG73">
-        <v>22.270049346344887</v>
+        <v>22.613849135906971</v>
       </c>
       <c r="CI73">
-        <v>27.143324300893848</v>
+        <v>29.253957265661104</v>
       </c>
       <c r="CK73">
-        <v>26.359955076794279</v>
+        <v>31.029730799782669</v>
       </c>
       <c r="CM73">
-        <v>29.987714729363773</v>
+        <v>34.216715623344562</v>
       </c>
       <c r="CO73">
-        <v>38.856986701328047</v>
+        <v>43.639241254529786</v>
       </c>
       <c r="CQ73">
-        <v>55.910501561925649</v>
+        <v>58.978152186389856</v>
       </c>
       <c r="CS73">
-        <v>64.375052867162893</v>
+        <v>66.664238269428196</v>
       </c>
       <c r="CU73">
-        <v>65.918780378894596</v>
+        <v>67.38735273544988</v>
       </c>
       <c r="CW73">
-        <v>68.581710336631772</v>
+        <v>69.130139847378572</v>
       </c>
     </row>
     <row r="74" spans="1:101" x14ac:dyDescent="0.25">
@@ -6843,10 +6807,10 @@
         <v>146</v>
       </c>
       <c r="C74" s="7">
-        <v>37712</v>
+        <v>37697</v>
       </c>
       <c r="F74" s="13">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="G74" t="s">
         <v>106</v>
@@ -6860,31 +6824,31 @@
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
       <c r="U74">
-        <v>341.37321490770455</v>
+        <v>279.40264957031496</v>
       </c>
       <c r="AB74">
-        <v>92.741828531482483</v>
+        <v>135.12584023274374</v>
       </c>
       <c r="AC74">
-        <v>1.0930179610660558</v>
+        <v>1.6312750689369722</v>
       </c>
       <c r="AI74">
-        <v>1.1785598562950653E-2</v>
+        <v>1.2072265868076956E-2</v>
       </c>
       <c r="AJ74">
-        <v>1.756725381973891E-2</v>
+        <v>1.5076837778112202E-2</v>
       </c>
       <c r="AK74">
-        <v>1.6292192415192568</v>
+        <v>2.0372703728201844</v>
       </c>
       <c r="AZ74">
-        <v>730.38715588683078</v>
+        <v>685.17875096619355</v>
       </c>
       <c r="BC74">
-        <v>1164.5021993260179</v>
+        <v>1099.7072407692522</v>
       </c>
       <c r="BE74">
-        <v>0.62720976938434203</v>
+        <v>0.6230555965848753</v>
       </c>
     </row>
     <row r="75" spans="1:101" x14ac:dyDescent="0.25">
@@ -6895,10 +6859,10 @@
         <v>146</v>
       </c>
       <c r="C75" s="7">
-        <v>37722</v>
-      </c>
-      <c r="F75" s="14">
-        <v>183</v>
+        <v>37698</v>
+      </c>
+      <c r="F75">
+        <v>159</v>
       </c>
       <c r="G75" t="s">
         <v>106</v>
@@ -6911,19 +6875,132 @@
       </c>
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
-      <c r="BF75">
+      <c r="CE75">
+        <v>399.40407529933975</v>
+      </c>
+      <c r="CG75">
+        <v>22.270049346344887</v>
+      </c>
+      <c r="CI75">
+        <v>27.143324300893848</v>
+      </c>
+      <c r="CK75">
+        <v>26.359955076794279</v>
+      </c>
+      <c r="CM75">
+        <v>29.987714729363773</v>
+      </c>
+      <c r="CO75">
+        <v>38.856986701328047</v>
+      </c>
+      <c r="CQ75">
+        <v>55.910501561925649</v>
+      </c>
+      <c r="CS75">
+        <v>64.375052867162893</v>
+      </c>
+      <c r="CU75">
+        <v>65.918780378894596</v>
+      </c>
+      <c r="CW75">
+        <v>68.581710336631772</v>
+      </c>
+    </row>
+    <row r="76" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>145</v>
+      </c>
+      <c r="B76" t="s">
+        <v>146</v>
+      </c>
+      <c r="C76" s="7">
+        <v>37712</v>
+      </c>
+      <c r="F76" s="13">
+        <v>173</v>
+      </c>
+      <c r="G76" t="s">
+        <v>106</v>
+      </c>
+      <c r="H76" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="I76" s="14">
+        <v>380</v>
+      </c>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="U76">
+        <v>341.37321490770455</v>
+      </c>
+      <c r="AB76">
+        <v>92.741828531482483</v>
+      </c>
+      <c r="AC76">
+        <v>1.0930179610660558</v>
+      </c>
+      <c r="AI76">
+        <v>1.1785598562950653E-2</v>
+      </c>
+      <c r="AJ76">
+        <v>1.756725381973891E-2</v>
+      </c>
+      <c r="AK76">
+        <v>1.6292192415192568</v>
+      </c>
+      <c r="AZ76">
+        <v>730.38715588683078</v>
+      </c>
+      <c r="BC76">
+        <v>1164.5021993260179</v>
+      </c>
+      <c r="BE76">
+        <v>0.62720976938434203</v>
+      </c>
+    </row>
+    <row r="77" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77" t="s">
+        <v>146</v>
+      </c>
+      <c r="C77" s="7">
+        <v>37722</v>
+      </c>
+      <c r="D77" s="1">
+        <v>9</v>
+      </c>
+      <c r="E77" t="s">
+        <v>53</v>
+      </c>
+      <c r="F77" s="14">
+        <v>183</v>
+      </c>
+      <c r="G77" t="s">
+        <v>106</v>
+      </c>
+      <c r="H77" s="14">
+        <v>28.6</v>
+      </c>
+      <c r="I77" s="14">
+        <v>380</v>
+      </c>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="BF77">
         <v>989.1681890731428</v>
       </c>
-      <c r="BG75">
+      <c r="BG77">
         <v>0.43895467403460303</v>
       </c>
-      <c r="BH75">
+      <c r="BH77">
         <v>434.2</v>
       </c>
-      <c r="BI75">
+      <c r="BI77">
         <v>532.5</v>
       </c>
-      <c r="BJ75">
+      <c r="BJ77">
         <v>19.127753303964756</v>
       </c>
     </row>
@@ -6944,7 +7021,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D4BD3FF-AE44-4ECA-9411-35AD6BB15F82}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7000,9 +7077,26 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1">
-        <v>148</v>
+        <v>148.30000000000001</v>
       </c>
       <c r="H2" s="1">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="1">
+        <v>59.7</v>
+      </c>
+      <c r="D3">
+        <v>79</v>
+      </c>
+      <c r="G3">
+        <v>146</v>
+      </c>
+      <c r="H3" s="1">
         <v>183</v>
       </c>
     </row>

</xml_diff>